<commit_message>
Correção da Base de Dados - Município Extinto
</commit_message>
<xml_diff>
--- a/lista1.xlsx
+++ b/lista1.xlsx
@@ -1432,1354 +1432,1354 @@
     <t>AP</t>
   </si>
   <si>
-    <t>[410754.0, 410500.0, 410630.0, 411275.0, 411670.0, 410530.0, 410405.0, 410930.0, 412855.0, 411065.0, 412090.0, 410305.0, 410820.0, 411345.0, 410712.0, 410460.0, 412382.0, 410975.0, 410335.0, 410345.0, 410480.0, 412785.0, 412402.0, 410105.0, 411005.0]</t>
-  </si>
-  <si>
-    <t>[250915.0, 251620.0, 251398.0, 251420.0, 251720.0, 250840.0, 251320.0, 251000.0, 250077.0]</t>
-  </si>
-  <si>
-    <t>[230690.0, 230600.0, 230760.0, 231080.0, 231310.0, 231150.0, 231250.0, 231123.0, 230070.0, 230680.0, 230427.0]</t>
-  </si>
-  <si>
-    <t>[270240.0, 270330.0, 270500.0, 270642.0, 270580.0, 270710.0, 270010.0]</t>
-  </si>
-  <si>
-    <t>[412800.0, 410755.0, 411400.0, 410250.0, 410770.0, 410390.0, 411295.0, 410655.0, 412065.0, 411680.0, 412720.0, 410170.0, 410300.0, 410045.0, 410430.0, 411080.0, 412110.0, 411220.0, 411610.0, 412250.0, 412135.0, 411880.0, 410860.0, 411373.0, 410750.0]</t>
-  </si>
-  <si>
-    <t>[251660.0, 250670.0, 250800.0, 250900.0, 250010.0, 251230.0, 251455.0]</t>
-  </si>
-  <si>
-    <t>[230400.0, 231170.0, 230800.0, 231200.0, 230050.0, 230435.0, 230820.0, 230310.0, 230450.0, 231220.0, 230580.0, 231095.0, 230465.0, 230990.0, 230610.0, 230490.0, 230365.0, 231390.0, 230880.0, 231395.0, 231280.0, 230900.0, 230520.0, 231290.0]</t>
-  </si>
-  <si>
-    <t>[410752.0, 412810.0, 412690.0, 411155.0, 410660.0, 411060.0, 412862.0, 410050.0, 411720.0, 411470.0, 412880.0, 410832.0, 410070.0, 410337.0, 410725.0, 410347.0, 411885.0, 410990.0, 411890.0, 411510.0, 412535.0]</t>
-  </si>
-  <si>
-    <t>[250720.0, 250690.0, 250790.0, 250760.0, 251275.0, 250380.0, 251500.0, 251310.0, 251150.0, 251120.0, 250640.0, 251445.0, 250680.0, 250940.0]</t>
-  </si>
-  <si>
-    <t>[230020.0, 230725.0, 230890.0, 230230.0, 230425.0, 230780.0, 230655.0]</t>
-  </si>
-  <si>
-    <t>[411040.0, 410560.0, 412610.0, 412260.0, 411300.0, 412680.0, 411240.0, 412555.0, 410550.0, 412790.0, 410910.0]</t>
-  </si>
-  <si>
-    <t>[251392.0, 251396.0, 250375.0, 251210.0, 251090.0, 250810.0]</t>
-  </si>
-  <si>
-    <t>[231360.0, 230530.0, 230500.0, 230340.0, 231340.0, 231410.0, 230423.0, 231230.0]</t>
-  </si>
-  <si>
-    <t>[411650.0, 412420.0, 410890.0, 411030.0, 411800.0, 412330.0, 412460.0, 412590.0, 410670.0, 411830.0, 412730.0, 411710.0, 411840.0, 411970.0, 412100.0, 411590.0, 412490.0, 410060.0, 412370.0, 410710.0, 411350.0, 410090.0, 412395.0, 411500.0, 412020.0, 411130.0, 411260.0, 412670.0]</t>
-  </si>
-  <si>
-    <t>[250403.0, 251272.0, 250890.0, 250730.0, 250930.0, 250710.0, 250905.0, 251290.0, 250523.0, 250140.0, 250527.0]</t>
-  </si>
-  <si>
-    <t>[230040.0, 231330.0, 231030.0, 230150.0]</t>
-  </si>
-  <si>
-    <t>[411520.0, 410115.0, 412040.0, 411410.0, 411160.0, 411640.0, 410780.0, 411420.0, 412830.0, 412450.0, 411810.0, 410790.0, 411690.0, 412340.0, 410810.0, 412360.0, 412625.0, 411090.0, 411480.0, 411740.0, 410590.0, 411360.0, 410210.0, 411750.0, 411110.0, 410730.0, 410220.0, 411630.0, 412530.0, 411000.0]</t>
-  </si>
-  <si>
-    <t>[250625.0, 251394.0, 250435.0, 250053.0, 250310.0, 250250.0, 250157.0, 251278.0, 250990.0, 251250.0, 250130.0, 251700.0, 251315.0, 250170.0]</t>
-  </si>
-  <si>
-    <t>[230560.0, 230565.0, 230410.0, 230860.0, 230125.0, 230930.0, 231126.0, 231320.0, 231100.0, 230940.0, 230590.0]</t>
-  </si>
-  <si>
-    <t>[411490.0, 412580.0, 410150.0, 410760.0, 411210.0, 410380.0, 411310.0, 410350.0, 410320.0, 411729.0, 412210.0, 412270.0, 410870.0, 411575.0, 410330.0, 410140.0, 411550.0]</t>
-  </si>
-  <si>
-    <t>[251200.0, 250400.0, 251650.0, 250850.0, 250215.0, 251240.0, 250920.0, 251050.0, 250610.0, 250770.0, 250135.0, 251385.0, 251610.0, 251675.0, 251580.0]</t>
-  </si>
-  <si>
-    <t>[230470.0, 230790.0, 230260.0, 230390.0, 230205.0]</t>
-  </si>
-  <si>
-    <t>[412033.0, 410370.0, 411270.0, 410510.0, 412050.0, 410920.0, 410280.0, 410800.0, 411190.0, 411965.0, 410190.0, 411600.0, 412240.0, 410080.0, 412000.0, 410980.0, 410340.0, 412650.0, 411370.0, 411380.0, 412667.0]</t>
-  </si>
-  <si>
-    <t>[230180.0, 230950.0, 230570.0, 231370.0, 230540.0, 230380.0, 230750.0]</t>
-  </si>
-  <si>
-    <t>[410240.0, 411660.0, 412430.0, 410640.0, 412310.0, 410010.0, 412190.0, 412320.0, 412840.0, 411700.0, 412470.0, 412600.0, 411721.0, 412620.0, 411340.0, 411100.0, 412640.0, 412130.0, 412390.0, 410600.0, 410110.0]</t>
-  </si>
-  <si>
-    <t>[230330.0, 230850.0, 230030.0, 231090.0, 230740.0, 230550.0, 231190.0, 230360.0, 230426.0, 231135.0]</t>
-  </si>
-  <si>
-    <t>[412290.0, 411920.0, 411280.0, 412180.0, 410900.0, 410775.0, 411290.0, 410270.0, 411170.0, 412070.0, 411180.0, 412850.0, 410970.0, 411230.0, 410470.0, 412780.0, 412400.0, 410610.0, 412660.0, 410360.0, 412410.0, 412540.0]</t>
-  </si>
-  <si>
-    <t>[230720.0, 231110.0, 230250.0, 230830.0, 230810.0, 231060.0, 230200.0, 230010.0, 230170.0]</t>
-  </si>
-  <si>
-    <t>[411620.0, 410950.0, 410120.0, 411820.0, 410960.0, 411570.0, 411995.0]</t>
-  </si>
-  <si>
-    <t>[230440.0, 230625.0, 230100.0, 230428.0]</t>
-  </si>
-  <si>
-    <t>[250180.0, 251370.0, 251530.0, 251276.0, 250860.0, 250060.0, 251597.0, 250320.0, 251190.0, 250910.0, 250490.0, 250300.0, 250750.0, 250460.0]</t>
-  </si>
-  <si>
-    <t>[270690.0, 270050.0, 270470.0, 270790.0, 270280.0, 270890.0, 270220.0, 270060.0, 270770.0, 270644.0, 270520.0, 270430.0]</t>
-  </si>
-  <si>
-    <t>[240770.0, 241420.0, 240140.0, 240910.0, 240780.0, 240660.0, 240790.0, 240920.0, 240420.0, 241320.0, 241330.0, 240180.0, 240820.0, 241470.0, 240830.0, 241220.0, 241350.0, 241480.0, 240980.0, 241500.0, 240220.0, 240350.0, 240615.0, 240620.0, 240630.0, 240120.0, 241150.0]</t>
-  </si>
-  <si>
-    <t>[410880.0, 410753.0, 411585.0, 412545.0, 411460.0, 411845.0, 411745.0, 412740.0, 412770.0, 411722.0, 412795.0, 411790.0, 411535.0, 412085.0, 410200.0, 410715.0, 412350.0, 412575.0]</t>
-  </si>
-  <si>
-    <t>[230080.0, 231400.0, 230920.0, 231210.0, 230060.0, 230160.0, 231120.0, 230130.0, 230420.0, 230430.0, 231195.0, 231325.0, 230270.0]</t>
-  </si>
-  <si>
-    <t>[412710.0, 412170.0, 410700.0, 412750.0, 411730.0, 412853.0, 411007.0]</t>
-  </si>
-  <si>
-    <t>[230730.0, 230190.0, 230480.0, 230320.0, 230710.0, 230840.0]</t>
-  </si>
-  <si>
-    <t>[412385.0, 410855.0, 410440.0, 410185.0, 412265.0, 411150.0, 411375.0, 411727.0, 411342.0, 411250.0, 412500.0, 410165.0, 411573.0, 412217.0, 411450.0, 410685.0]</t>
-  </si>
-  <si>
-    <t>[230945.0, 230523.0, 230220.0, 231085.0, 230350.0, 230960.0, 230395.0]</t>
-  </si>
-  <si>
-    <t>[411910.0, 412550.0, 411915.0, 410765.0, 410520.0, 410400.0, 410020.0, 411430.0, 410410.0, 410030.0, 411950.0, 412080.0, 410420.0, 410040.0, 410425.0, 411320.0, 412220.0, 412863.0, 410690.0, 410180.0, 412230.0, 410310.0, 410580.0, 412760.0, 412120.0, 412788.0, 411125.0, 410230.0, 410620.0]</t>
-  </si>
-  <si>
-    <t>[250630.0, 251274.0, 251640.0, 250520.0, 251160.0, 250270.0, 251170.0, 250150.0, 251560.0, 251180.0, 250415.0, 250050.0, 250820.0, 251590.0, 251593.0, 250570.0, 250190.0, 251600.0, 250580.0, 250080.0, 250980.0, 250855.0, 250350.0, 250100.0, 250360.0]</t>
-  </si>
-  <si>
-    <t>[230370.0, 230630.0, 231335.0, 231240.0, 230090.0, 231020.0, 230460.0, 231025.0, 231260.0, 231070.0]</t>
-  </si>
-  <si>
-    <t>[270850.0, 270730.0, 270510.0, 270350.0, 270450.0, 270740.0, 270870.0, 270360.0, 270650.0]</t>
-  </si>
-  <si>
-    <t>[240800.0, 240130.0, 240100.0, 240230.0, 240520.0, 240430.0, 240110.0, 241105.0, 240370.0, 240440.0, 241460.0, 240145.0, 241335.0, 240760.0]</t>
-  </si>
-  <si>
-    <t>[411200.0, 410465.0, 411140.0, 411940.0, 411770.0, 411050.0, 412010.0, 410160.0, 412630.0, 411990.0, 410490.0, 412510.0]</t>
-  </si>
-  <si>
-    <t>[251270.0, 250950.0, 250120.0, 250057.0, 250090.0, 250600.0, 250830.0, 250030.0, 250933.0, 251510.0, 250040.0, 250110.0]</t>
-  </si>
-  <si>
-    <t>[231010.0, 230765.0, 230015.0, 230770.0, 230195.0, 231160.0, 230970.0, 230495.0]</t>
-  </si>
-  <si>
-    <t>[270560.0, 270210.0, 270380.0, 270830.0, 270930.0, 270390.0, 270135.0, 270550.0, 270810.0, 270300.0, 270110.0]</t>
-  </si>
-  <si>
-    <t>[240260.0, 241160.0, 241040.0, 240410.0, 240670.0, 240030.0, 241440.0, 240160.0, 240550.0, 240950.0, 240185.0, 240190.0, 240960.0, 241090.0, 240450.0, 240580.0, 240970.0, 240460.0, 240720.0, 241255.0, 241390.0, 240750.0, 240880.0, 241010.0, 240510.0, 240895.0]</t>
-  </si>
-  <si>
-    <t>[411010.0, 412200.0, 411020.0, 411390.0, 410895.0, 410773.0, 412150.0, 412700.0, 411070.0]</t>
-  </si>
-  <si>
-    <t>[251010.0, 250500.0, 251140.0, 251110.0, 250535.0, 250153.0, 250510.0, 250160.0, 251540.0, 251030.0, 250620.0, 251615.0]</t>
-  </si>
-  <si>
-    <t>[230210.0, 230980.0, 230120.0, 230510.0, 230290.0, 230650.0, 230140.0, 230910.0]</t>
-  </si>
-  <si>
-    <t>[270660.0, 270490.0, 270760.0, 270700.0, 270190.0, 270130.0, 270040.0, 270170.0, 270940.0]</t>
-  </si>
-  <si>
-    <t>[241415.0, 240650.0, 240010.0, 240270.0, 241300.0, 241430.0, 241180.0, 240165.0, 240300.0, 240560.0, 240310.0, 241210.0, 240570.0, 241340.0, 240200.0, 240850.0, 240340.0, 241240.0, 240480.0, 240610.0, 240240.0, 241140.0, 241142.0, 240890.0, 240380.0]</t>
-  </si>
-  <si>
-    <t>[411780.0, 412175.0, 411545.0, 411930.0, 410395.0, 412060.0, 412215.0, 411960.0, 411705.0, 410940.0, 411325.0, 410304.0, 412865.0, 411330.0, 410442.0, 410445.0, 410845.0, 412015.0, 410865.0, 412796.0]</t>
-  </si>
-  <si>
-    <t>[251520.0, 251065.0, 250970.0, 250470.0, 250407.0, 251400.0, 251630.0, 251410.0, 251220.0, 250485.0, 250390.0, 251060.0, 251480.0, 250073.0, 250650.0, 251740.0, 251550.0]</t>
-  </si>
-  <si>
-    <t>[230240.0, 231040.0, 230660.0, 230280.0, 230763.0, 230300.0]</t>
-  </si>
-  <si>
-    <t>[270400.0, 270915.0, 270020.0, 270140.0, 270860.0, 270100.0, 270780.0]</t>
-  </si>
-  <si>
-    <t>[240640.0, 241030.0, 241290.0, 241170.0, 240530.0, 240150.0, 240280.0, 240540.0, 241310.0, 240933.0, 240680.0, 240170.0, 241230.0, 240210.0, 241110.0, 241370.0, 241120.0, 241260.0, 240500.0, 241270.0, 241400.0]</t>
-  </si>
-  <si>
-    <t>[412030.0, 410850.0, 412560.0, 410290.0, 410130.0, 412820.0, 411860.0, 410680.0, 411870.0]</t>
-  </si>
-  <si>
-    <t>[250880.0, 250115.0, 251670.0, 250780.0, 251300.0, 250540.0, 251440.0, 250420.0, 250550.0, 250939.0, 251070.0, 251710.0, 251460.0, 251080.0, 251340.0, 251470.0, 250450.0, 250590.0, 251490.0, 250340.0, 250355.0, 251380.0, 250870.0, 251260.0]</t>
-  </si>
-  <si>
-    <t>[231355.0, 231375.0, 230640.0, 231380.0, 230837.0, 231350.0, 230075.0]</t>
-  </si>
-  <si>
-    <t>[270820.0, 270375.0, 270670.0, 270320.0, 270270.0, 270230.0, 270680.0, 270750.0]</t>
-  </si>
-  <si>
-    <t>[241410.0, 240390.0, 240400.0, 241050.0, 240930.0, 240290.0, 241060.0, 241190.0, 240040.0, 241450.0, 240940.0, 241070.0, 240690.0, 240050.0, 241080.0, 240700.0, 240060.0, 240320.0, 241475.0, 240840.0, 240330.0, 241355.0, 241100.0, 240590.0, 241360.0, 241490.0, 240725.0, 240600.0, 240090.0, 240730.0, 240860.0, 241250.0, 241380.0, 240740.0, 241000.0, 240490.0, 241020.0]</t>
-  </si>
-  <si>
-    <t>[412480.0, 412870.0, 410570.0, 411530.0, 410540.0, 411850.0, 411120.0, 411760.0, 410322.0, 412627.0, 411440.0, 410965.0, 410645.0, 412665.0, 410650.0]</t>
-  </si>
-  <si>
-    <t>[250560.0, 251360.0, 250210.0, 250530.0, 250020.0, 251040.0, 250660.0, 251335.0, 250440.0, 251430.0, 251020.0, 250700.0, 250480.0, 251570.0, 250260.0, 251350.0, 251130.0, 251100.0]</t>
-  </si>
-  <si>
-    <t>[230620.0, 230445.0, 230110.0, 230535.0]</t>
-  </si>
-  <si>
-    <t>[270880.0, 270370.0, 270340.0, 270150.0, 270920.0, 270440.0, 270090.0, 270410.0, 270030.0, 270290.0, 270420.0, 270260.0, 270070.0, 270200.0, 270235.0, 270910.0, 270590.0]</t>
-  </si>
-  <si>
-    <t>[240325.0, 240710.0, 240360.0, 240810.0, 241200.0]</t>
-  </si>
-  <si>
-    <t>[412160.0, 412035.0, 412300.0, 411540.0, 410260.0, 411925.0, 412440.0, 410657.0, 410785.0, 410275.0, 411435.0, 411695.0, 412860.0, 410302.0, 410315.0, 411980.0, 411725.0, 410450.0, 410840.0, 412380.0, 410720.0, 412520.0, 412140.0, 410100.0, 410740.0, 412280.0, 411900.0]</t>
-  </si>
-  <si>
-    <t>[250280.0, 251465.0, 250430.0, 251280.0, 250290.0, 250740.0, 250230.0, 250200.0, 250937.0, 251390.0]</t>
-  </si>
-  <si>
-    <t>[231300.0, 231140.0, 231270.0, 230533.0, 230185.0, 231050.0, 230835.0, 230393.0, 231130.0, 230526.0]</t>
-  </si>
-  <si>
-    <t>[270080.0, 270530.0, 270630.0, 270310.0, 270120.0, 270255.0, 270480.0, 270900.0]</t>
-  </si>
-  <si>
-    <t>[241280.0, 241025.0, 240485.0, 240870.0, 240070.0, 241445.0, 240080.0, 240020.0, 240470.0, 240375.0, 240250.0, 240990.0]</t>
-  </si>
-  <si>
-    <t>[411560.0, 410830.0, 412405.0, 411605.0, 411095.0, 412570.0, 412635.0, 411580.0, 412125.0]</t>
-  </si>
-  <si>
-    <t>[250240.0, 251680.0, 250370.0, 251330.0, 251203.0, 251365.0, 251207.0, 250410.0, 251690.0, 250220.0, 250960.0, 251450.0, 250070.0, 250330.0, 250205.0]</t>
-  </si>
-  <si>
-    <t>[230700.0, 231180.0, 230670.0, 230870.0, 231000.0]</t>
-  </si>
-  <si>
-    <t>[270720.0, 270180.0, 270600.0, 270570.0, 270250.0, 270540.0, 270895.0, 270800.0, 270160.0, 270610.0, 270640.0, 270620.0, 270840.0, 270460.0]</t>
-  </si>
-  <si>
-    <t>[352740.0, 354085.0, 354470.0, 354510.0, 351600.0, 352080.0, 353490.0, 353460.0, 352890.0, 350010.0]</t>
-  </si>
-  <si>
-    <t>[261440.0, 261153.0, 260770.0, 261280.0, 260390.0, 260710.0, 260010.0, 261360.0, 260690.0, 261460.0, 261590.0, 260250.0]</t>
-  </si>
-  <si>
-    <t>[291650.0, 291590.0, 292970.0, 291370.0, 291050.0, 290220.0, 291790.0, 290700.0, 290960.0, 292330.0, 290030.0, 290190.0, 291060.0, 290070.0, 292410.0, 292700.0, 290205.0, 290750.0]</t>
-  </si>
-  <si>
-    <t>[314720.0, 315170.0, 310530.0, 312520.0, 313900.0, 311470.0, 312240.0, 310160.0, 316690.0, 311160.0, 310200.0, 310840.0, 311130.0, 310430.0, 311100.0, 311710.0]</t>
-  </si>
-  <si>
-    <t>[313600.0, 315710.0, 315810.0, 314055.0, 315660.0, 313580.0, 312560.0, 313650.0, 314675.0, 315510.0, 310520.0, 313470.0, 316030.0, 310170.0]</t>
-  </si>
-  <si>
-    <t>[352130.0, 353190.0, 353360.0, 353430.0, 354490.0, 354940.0]</t>
-  </si>
-  <si>
-    <t>[350820.0, 352410.0, 352010.0, 352970.0, 351770.0, 350300.0]</t>
-  </si>
-  <si>
-    <t>[352160.0, 353540.0, 353160.0, 353640.0, 353480.0, 351440.0, 354930.0, 355510.0, 354710.0, 352600.0, 351580.0, 353310.0]</t>
-  </si>
-  <si>
-    <t>[353920.0, 350080.0, 354830.0, 354323.0, 351512.0, 352920.0, 350240.0, 351530.0, 350890.0, 350130.0, 352060.0, 355390.0, 354240.0, 353220.0, 354120.0, 354770.0, 355290.0, 354140.0, 354550.0]</t>
-  </si>
-  <si>
-    <t>[120025.0, 120010.0, 120005.0, 120070.0]</t>
-  </si>
-  <si>
-    <t>[354220.0, 352560.0, 351990.0, 354170.0, 353215.0]</t>
-  </si>
-  <si>
-    <t>[130370.0, 130020.0, 130406.0, 130060.0, 130160.0, 130390.0, 130423.0, 130006.0, 130230.0]</t>
-  </si>
-  <si>
-    <t>[510080.0, 510629.0, 510279.0, 510025.0, 510895.0, 510615.0]</t>
-  </si>
-  <si>
-    <t>[420800.0, 420770.0, 421960.0, 420075.0, 420780.0, 421260.0, 420430.0, 421390.0, 421750.0, 420760.0, 420985.0, 421310.0, 420127.0]</t>
-  </si>
-  <si>
-    <t>[420740.0, 421780.0, 421270.0, 421400.0, 421530.0, 420510.0, 421920.0, 421410.0, 421935.0, 420915.0, 420020.0, 421940.0, 420285.0, 420030.0, 421567.0, 420419.0, 421450.0, 420690.0, 420180.0, 421460.0, 420950.0, 421085.0, 420190.0, 421860.0, 421480.0, 420850.0, 421370.0, 420990.0]</t>
-  </si>
-  <si>
-    <t>[353560.0, 350850.0, 354600.0, 352490.0, 354990.0, 353170.0, 352020.0, 352440.0]</t>
-  </si>
-  <si>
-    <t>[420480.0, 421005.0, 420757.0, 421790.0, 421540.0, 421930.0, 421550.0, 421300.0, 421440.0, 420160.0, 421825.0, 420675.0, 420550.0, 420555.0, 420300.0, 421070.0, 421335.0, 420315.0, 421605.0, 420970.0]</t>
-  </si>
-  <si>
-    <t>[354500.0, 353060.0, 354680.0, 350660.0, 351880.0, 355250.0, 351570.0, 351830.0, 352310.0, 350390.0, 353980.0]</t>
-  </si>
-  <si>
-    <t>[316000.0, 310150.0, 315110.0, 312460.0, 317210.0]</t>
-  </si>
-  <si>
-    <t>[171360.0, 172065.0, 170370.0, 170755.0, 170980.0, 171270.0, 171820.0, 170510.0, 171790.0, 171890.0, 171700.0, 171420.0, 171550.0]</t>
-  </si>
-  <si>
-    <t>[354340.0, 354750.0, 355140.0, 354760.0, 351885.0, 351310.0, 355150.0, 355090.0, 352760.0, 352510.0]</t>
-  </si>
-  <si>
-    <t>[280320.0, 280030.0, 280200.0, 280360.0, 280650.0, 280590.0, 280060.0, 280670.0]</t>
-  </si>
-  <si>
-    <t>[150304.0, 150658.0, 150840.0, 150276.0, 150555.0, 150730.0, 150125.0, 150670.0, 150543.0, 150034.0, 150613.0, 150775.0, 150808.0, 150616.0, 150270.0]</t>
-  </si>
-  <si>
-    <t>[510860.0, 510735.0, 510677.0, 510774.0, 510777.0, 510269.0, 510335.0]</t>
-  </si>
-  <si>
-    <t>[353930.0, 351220.0, 350330.0, 354620.0, 352670.0]</t>
-  </si>
-  <si>
-    <t>[310400.0, 314980.0, 315300.0, 314920.0, 316810.0, 311150.0, 312950.0, 315770.0]</t>
-  </si>
-  <si>
-    <t>[310340.0, 317160.0, 313545.0, 312650.0, 311950.0, 310650.0]</t>
-  </si>
-  <si>
-    <t>[261600.0, 261410.0, 260805.0, 261480.0, 261580.0, 261100.0, 260915.0, 260660.0, 260280.0, 261080.0, 260120.0, 260700.0, 260510.0]</t>
-  </si>
-  <si>
-    <t>[350720.0, 350400.0, 351330.0, 355395.0, 353530.0, 353550.0, 352880.0, 353970.0, 353715.0, 352790.0, 351000.0, 351610.0]</t>
-  </si>
-  <si>
-    <t>[211085.0, 210542.0, 211153.0, 210005.0, 211285.0, 210325.0, 210232.0, 210203.0]</t>
-  </si>
-  <si>
-    <t>[211300.0, 211140.0, 210215.0, 210120.0, 210635.0, 210355.0, 210740.0, 210040.0, 210810.0, 210590.0, 210207.0]</t>
-  </si>
-  <si>
-    <t>[330380.0, 330010.0, 330260.0]</t>
-  </si>
-  <si>
-    <t>[353080.0, 355730.0, 352260.0, 353070.0]</t>
-  </si>
-  <si>
-    <t>[510620.0, 510340.0, 510010.0, 510650.0, 510160.0, 510610.0, 510645.0, 510300.0, 510840.0, 510490.0, 510780.0]</t>
-  </si>
-  <si>
-    <t>[330020.0, 330023.0, 330025.0, 330187.0, 330130.0, 330452.0, 330070.0, 330550.0, 330520.0]</t>
-  </si>
-  <si>
-    <t>[353760.0, 354850.0, 350635.0, 352210.0, 354100.0, 351350.0, 353110.0, 355100.0, 351870.0]</t>
-  </si>
-  <si>
-    <t>[120032.0, 120001.0, 120034.0, 120038.0, 120040.0, 120043.0, 120045.0, 120013.0, 120080.0, 120017.0, 120050.0]</t>
-  </si>
-  <si>
-    <t>[130050.0, 130340.0, 130290.0, 130068.0, 130300.0]</t>
-  </si>
-  <si>
-    <t>[150145.0, 150050.0, 150530.0, 150565.0, 150600.0, 150475.0, 150285.0, 150510.0, 150797.0, 150480.0, 150390.0, 150040.0, 150300.0, 150680.0]</t>
-  </si>
-  <si>
-    <t>[211200.0, 210050.0, 210725.0, 210950.0, 210407.0, 211080.0, 210409.0, 210410.0, 210610.0, 211157.0, 211160.0, 210970.0, 210140.0]</t>
-  </si>
-  <si>
-    <t>[310560.0, 310210.0, 315940.0, 314660.0, 316620.0, 312940.0, 311630.0, 315440.0, 315730.0, 310163.0, 311220.0, 310290.0, 312150.0, 311320.0, 315870.0]</t>
-  </si>
-  <si>
-    <t>[210535.0, 210408.0, 210095.0, 210160.0, 210480.0, 210547.0]</t>
-  </si>
-  <si>
-    <t>[293345.0, 293090.0, 291110.0, 290970.0, 292840.0, 290440.0, 290250.0, 292620.0, 292045.0, 290940.0, 290320.0, 291955.0, 290740.0, 292890.0, 290140.0]</t>
-  </si>
-  <si>
-    <t>[352800.0, 353890.0, 350340.0, 351910.0, 353670.0, 352680.0, 353657.0, 354250.0, 350470.0, 350600.0, 352750.0, 350830.0, 353940.0, 350070.0, 350745.0, 351450.0, 350430.0, 354110.0]</t>
-  </si>
-  <si>
-    <t>[316830.0, 315780.0, 315460.0, 310620.0, 310640.0, 314480.0, 313460.0, 315670.0, 314230.0, 311000.0, 315480.0, 313660.0, 315390.0]</t>
-  </si>
-  <si>
-    <t>[315040.0, 313665.0, 316292.0, 312410.0, 315530.0, 310670.0, 313010.0, 310900.0, 314070.0, 312600.0, 310810.0, 312060.0, 314015.0]</t>
-  </si>
-  <si>
-    <t>[170380.0, 170382.0, 170255.0, 171280.0, 170389.0, 171430.0, 170030.0, 172080.0, 170290.0, 171830.0, 171070.0, 171855.0, 172120.0, 172000.0, 171880.0, 172010.0, 170220.0, 171245.0, 170740.0, 172020.0, 170100.0, 171380.0, 170105.0, 172030.0]</t>
-  </si>
-  <si>
-    <t>[313640.0, 310730.0, 314545.0, 312660.0, 312825.0, 312380.0]</t>
-  </si>
-  <si>
-    <t>[314240.0, 312320.0, 314050.0, 310740.0, 316660.0, 312470.0, 313880.0]</t>
-  </si>
-  <si>
-    <t>[353860.0, 352550.0, 355495.0, 350760.0, 355210.0, 350410.0, 353680.0, 355635.0, 350710.0, 353240.0, 353820.0]</t>
-  </si>
-  <si>
-    <t>[317090.0, 316420.0, 312965.0, 317000.0, 313865.0, 311115.0, 313868.0, 310860.0, 316110.0, 313005.0, 316240.0, 315057.0, 314795.0, 317052.0, 313535.0]</t>
-  </si>
-  <si>
-    <t>[290050.0, 292360.0, 291720.0, 291980.0, 291860.0, 291220.0, 290200.0, 290460.0, 291250.0, 292670.0, 292030.0, 290880.0, 291010.0, 290755.0, 292690.0, 291165.0, 290280.0, 290410.0, 293100.0, 291950.0]</t>
-  </si>
-  <si>
-    <t>[110018.0, 110147.0, 110148.0, 110120.0, 110004.0, 110009.0]</t>
-  </si>
-  <si>
-    <t>[292100.0, 292520.0, 290570.0, 290860.0, 293070.0, 291005.0]</t>
-  </si>
-  <si>
-    <t>[310080.0, 311200.0, 311040.0, 315880.0, 311120.0, 312020.0, 311190.0]</t>
-  </si>
-  <si>
-    <t>[500740.0, 500490.0, 500110.0, 500750.0, 500627.0, 500500.0, 500640.0, 500769.0, 500260.0, 500390.0, 500270.0, 500790.0, 500150.0, 500280.0, 500025.0, 500793.0, 500410.0, 500540.0, 500800.0, 500295.0, 500560.0, 500690.0, 500220.0, 500310.0, 500580.0, 500325.0, 500070.0, 500710.0, 500330.0, 500210.0, 500215.0, 500600.0, 500730.0, 500348.0]</t>
-  </si>
-  <si>
-    <t>[170720.0, 171845.0, 170310.0, 171750.0, 170025.0, 171370.0, 171500.0, 170190.0, 171250.0, 170610.0, 170390.0, 171190.0, 170710.0, 171610.0, 170460.0]</t>
-  </si>
-  <si>
-    <t>[171200.0, 171330.0, 171875.0, 172100.0, 171240.0, 170825.0, 172110.0, 172015.0, 171510.0, 171320.0, 170110.0, 171195.0, 171900.0, 171870.0]</t>
-  </si>
-  <si>
-    <t>[150497.0, 150370.0, 150563.0, 150277.0, 150215.0, 150553.0, 150157.0, 150420.0, 150293.0, 150549.0, 150295.0, 150745.0, 150618.0, 150715.0, 150013.0, 150750.0, 150175.0]</t>
-  </si>
-  <si>
-    <t>[311330.0, 311010.0, 312420.0, 312200.0, 311210.0, 314587.0, 312530.0, 312595.0, 314900.0, 316920.0, 314875.0]</t>
-  </si>
-  <si>
-    <t>[312385.0, 313090.0, 316447.0, 317057.0, 315015.0, 311340.0, 315725.0, 315935.0, 317005.0, 316095.0, 317115.0, 310780.0, 313055.0]</t>
-  </si>
-  <si>
-    <t>[421760.0, 420545.0, 420960.0, 421120.0, 421160.0, 420425.0, 421835.0, 421900.0, 420460.0, 422000.0, 421170.0, 420700.0]</t>
-  </si>
-  <si>
-    <t>[220194.0, 220675.0, 220260.0, 220551.0, 220105.0, 220202.0, 221065.0, 220205.0, 220527.0, 221040.0, 220271.0, 220177.0, 220695.0, 220220.0, 220990.0]</t>
-  </si>
-  <si>
-    <t>[261120.0, 261250.0, 260230.0, 260500.0, 261270.0, 261020.0, 260640.0, 260130.0, 260260.0, 261540.0, 261170.0, 261300.0, 260410.0, 260030.0, 261310.0, 260800.0, 260670.0, 260170.0, 261200.0, 261330.0, 260310.0, 260060.0, 260190.0, 261470.0, 261090.0, 260580.0, 260840.0, 260080.0, 261620.0, 261240.0, 261500.0, 260350.0]</t>
-  </si>
-  <si>
-    <t>[311240.0, 312970.0, 312120.0, 311510.0, 311640.0]</t>
-  </si>
-  <si>
-    <t>[354560.0, 351492.0, 351110.0, 351495.0, 351120.0, 355600.0, 353810.0, 352150.0, 353570.0, 350370.0, 353325.0, 354480.0, 355260.0, 352190.0, 353350.0, 351560.0, 353510.0, 353900.0, 352885.0]</t>
-  </si>
-  <si>
-    <t>[211107.0, 210340.0, 210220.0, 210030.0, 210390.0, 210010.0, 210300.0]</t>
-  </si>
-  <si>
-    <t>[521990.0, 520460.0, 521500.0, 522140.0, 520870.0, 520360.0, 521000.0, 520880.0, 521140.0, 521910.0, 520130.0, 521540.0, 520005.0, 520520.0, 521680.0, 520920.0, 520280.0, 521950.0, 520160.0, 521440.0, 521056.0, 520680.0, 521450.0, 522100.0, 521205.0, 521973.0]</t>
-  </si>
-  <si>
-    <t>[110180.0, 110025.0, 110155.0, 110143.0, 110175.0, 110032.0, 110160.0, 110034.0, 110130.0, 110100.0, 110170.0, 110011.0, 110012.0, 110015.0]</t>
-  </si>
-  <si>
-    <t>[320515.0, 320517.0, 320390.0, 320013.0, 320400.0, 320016.0, 320405.0, 320150.0, 320410.0, 320160.0, 320035.0, 320425.0, 320305.0, 320435.0, 320320.0, 320330.0, 320335.0, 320080.0, 320465.0, 320210.0, 320470.0, 320090.0, 320350.0, 320225.0, 320100.0, 320360.0, 320490.0, 320495.0, 320501.0]</t>
-  </si>
-  <si>
-    <t>[353286.0, 350280.0, 354440.0, 351820.0, 355630.0, 350640.0, 353330.0, 351890.0, 350420.0, 354805.0, 350620.0]</t>
-  </si>
-  <si>
-    <t>[354690.0, 354370.0, 351685.0, 350670.0, 350320.0, 355475.0, 353205.0, 350170.0]</t>
-  </si>
-  <si>
-    <t>[510050.0, 510600.0, 510890.0, 510730.0, 510350.0, 510770.0, 510590.0]</t>
-  </si>
-  <si>
-    <t>[140002.0, 140005.0, 140070.0, 140040.0, 140010.0, 140045.0, 140015.0, 140017.0, 140030.0]</t>
-  </si>
-  <si>
-    <t>[355270.0, 353290.0, 352270.0, 350740.0, 351960.0]</t>
-  </si>
-  <si>
-    <t>[520455.0, 520970.0, 520330.0, 521230.0, 520735.0, 520355.0, 520995.0, 520740.0, 522026.0, 521770.0, 521260.0, 520630.0, 521530.0, 522045.0, 520650.0, 520140.0, 522060.0, 522190.0, 521170.0, 522200.0, 522205.0, 520545.0, 521710.0, 521839.0, 520180.0]</t>
-  </si>
-  <si>
-    <t>[330370.0, 330180.0, 330022.0, 330600.0, 330280.0, 330540.0, 330095.0, 330385.0, 330290.0, 330360.0, 330620.0]</t>
-  </si>
-  <si>
-    <t>[171650.0, 171665.0, 171670.0, 170410.0, 171050.0, 171180.0, 171570.0, 170930.0, 170550.0, 171840.0, 170305.0, 171850.0, 170830.0, 170320.0, 171090.0, 170330.0, 172125.0, 172130.0, 171110.0, 170600.0, 171888.0, 170230.0, 170360.0]</t>
-  </si>
-  <si>
-    <t>[220930.0, 220290.0, 221062.0, 220552.0, 220300.0, 220045.0, 220310.0, 220440.0, 220190.0, 220320.0, 220323.0, 220975.0, 220740.0, 220870.0, 220360.0, 220110.0, 220885.0, 220760.0, 220130.0, 220275.0, 220660.0, 220920.0, 220665.0]</t>
-  </si>
-  <si>
-    <t>[210080.0, 210210.0, 211010.0, 210630.0, 210090.0, 210667.0, 211023.0, 210320.0, 210640.0, 211250.0, 211060.0, 210805.0, 210015.0]</t>
-  </si>
-  <si>
-    <t>[355200.0, 351840.0, 351360.0, 350250.0, 350315.0, 351340.0, 350860.0, 350350.0, 354190.0, 352720.0, 354960.0, 350995.0, 352660.0, 353850.0, 350490.0, 354075.0, 354430.0]</t>
-  </si>
-  <si>
-    <t>[353120.0, 350050.0, 350190.0, 355160.0, 352700.0]</t>
-  </si>
-  <si>
-    <t>[220545.0, 220680.0, 220557.0, 220830.0, 220196.0, 220580.0, 220840.0, 220585.0, 220850.0, 220342.0, 220217.0, 220987.0, 220610.0, 220997.0, 221005.0, 220240.0, 220370.0, 220120.0, 220635.0, 220150.0, 220790.0, 220667.0, 220540.0]</t>
-  </si>
-  <si>
-    <t>[211210.0, 211150.0, 210360.0, 210330.0, 210043.0, 210845.0]</t>
-  </si>
-  <si>
-    <t>[110146.0, 110092.0, 110030.0, 110003.0, 110005.0, 110006.0, 110007.0]</t>
-  </si>
-  <si>
-    <t>[313540.0, 312390.0, 312140.0, 311800.0, 316090.0, 314590.0]</t>
-  </si>
-  <si>
-    <t>[315520.0, 311490.0, 315910.0, 315080.0, 312040.0, 313390.0, 311310.0, 315380.0, 311540.0, 311830.0, 316600.0, 313790.0]</t>
-  </si>
-  <si>
-    <t>[355520.0, 352770.0, 353730.0, 351650.0, 351710.0, 350440.0, 353770.0, 350510.0, 350650.0, 350770.0, 351250.0, 352725.0, 351190.0, 350775.0, 354840.0, 350810.0, 350110.0]</t>
-  </si>
-  <si>
-    <t>[316553.0, 312980.0, 311860.0]</t>
-  </si>
-  <si>
-    <t>[316225.0, 313730.0, 311880.0, 316265.0, 313560.0]</t>
-  </si>
-  <si>
-    <t>[351430.0, 354890.0, 351370.0, 354290.0, 354070.0, 351930.0]</t>
-  </si>
-  <si>
-    <t>[312000.0, 311940.0, 316870.0, 315053.0, 314030.0, 313500.0, 312180.0, 310300.0]</t>
-  </si>
-  <si>
-    <t>[500520.0, 500320.0]</t>
-  </si>
-  <si>
-    <t>[292960.0, 290980.0, 290820.0, 292900.0, 292230.0, 290485.0, 291160.0, 290490.0, 292060.0]</t>
-  </si>
-  <si>
-    <t>[311910.0, 316935.0, 310920.0, 314250.0, 310480.0, 315320.0, 313110.0, 314360.0, 312570.0, 312090.0, 316060.0]</t>
-  </si>
-  <si>
-    <t>[312160.0, 311680.0, 313250.0, 311810.0, 312100.0, 315330.0, 312550.0, 312010.0, 316590.0, 311350.0, 312760.0, 312540.0]</t>
-  </si>
-  <si>
-    <t>[530010.0]</t>
-  </si>
-  <si>
-    <t>[312230.0, 313350.0, 311660.0, 316460.0, 316180.0, 310390.0, 314970.0, 311420.0]</t>
-  </si>
-  <si>
-    <t>[500480.0, 500620.0, 500240.0, 500625.0, 500370.0, 500375.0, 500635.0, 500380.0, 500124.0, 500510.0, 500770.0, 500515.0, 500525.0, 500400.0, 500660.0, 500795.0, 500797.0, 500430.0, 500568.0, 500570.0, 500315.0, 500060.0, 500450.0, 500840.0, 500200.0, 500460.0, 500720.0, 500080.0, 500085.0, 500470.0, 500345.0, 500090.0, 500350.0]</t>
-  </si>
-  <si>
-    <t>[521760.0, 520800.0, 522220.0, 522000.0, 520017.0, 520400.0, 520790.0, 520060.0]</t>
-  </si>
-  <si>
-    <t>[521250.0, 520549.0, 522185.0, 520620.0, 521523.0, 521975.0, 520025.0]</t>
-  </si>
-  <si>
-    <t>[220160.0, 220672.0, 220550.0, 220040.0, 220554.0, 220555.0, 220558.0, 220945.0, 220050.0, 220060.0, 220325.0, 220710.0, 220330.0, 220460.0, 221100.0, 220980.0, 221110.0, 220620.0, 220750.0, 220880.0, 220630.0, 220640.0, 220775.0, 220010.0, 220779.0, 220140.0, 220525.0, 220273.0, 220020.0, 221050.0, 220030.0]</t>
-  </si>
-  <si>
-    <t>[520480.0, 521920.0, 520450.0, 522180.0, 521480.0, 521290.0, 521740.0, 521580.0, 520590.0, 521550.0, 521010.0, 520850.0, 520690.0, 520660.0, 522130.0, 521878.0, 520120.0, 520510.0]</t>
-  </si>
-  <si>
-    <t>[280067.0, 280040.0, 280170.0, 280300.0, 280750.0, 280210.0, 280510.0, 280630.0, 280280.0, 280760.0]</t>
-  </si>
-  <si>
-    <t>[420490.0, 421520.0, 420500.0, 420765.0, 421535.0, 420640.0, 420257.0, 421795.0, 421670.0, 420775.0, 421415.0, 421555.0, 420660.0, 420535.0, 421050.0, 421568.0, 421200.0, 421715.0, 421720.0, 421730.0, 421090.0, 421223.0, 420840.0, 421100.0, 420080.0, 420208.0, 420209.0, 421875.0, 420215.0, 421625.0]</t>
-  </si>
-  <si>
-    <t>[353830.0, 354150.0, 352870.0, 354130.0, 350910.0]</t>
-  </si>
-  <si>
-    <t>[420195.0, 421380.0, 421125.0, 420870.0, 420519.0, 421640.0, 421225.0, 421770.0, 420140.0, 420207.0, 421040.0, 421810.0, 421880.0, 421080.0, 421565.0]</t>
-  </si>
-  <si>
-    <t>[291330.0, 291080.0, 292750.0, 292880.0, 293140.0, 292630.0, 290850.0, 293040.0, 292273.0, 293170.0, 291380.0, 291125.0, 292405.0, 290110.0, 292930.0, 291400.0, 290890.0, 290170.0, 290640.0, 290260.0, 292830.0, 290150.0, 292465.0, 292210.0, 292595.0, 293110.0, 291450.0, 290685.0]</t>
-  </si>
-  <si>
-    <t>[351520.0, 352960.0, 353475.0, 352070.0, 353000.0, 354920.0, 355530.0, 354925.0, 354040.0, 352820.0, 351800.0, 353690.0, 351550.0]</t>
-  </si>
-  <si>
-    <t>[312610.0, 313030.0, 311980.0, 310510.0, 314130.0, 316820.0, 314650.0, 311995.0]</t>
-  </si>
-  <si>
-    <t>[420320.0, 421280.0, 421250.0, 421350.0, 420710.0, 420200.0, 421000.0, 421130.0, 420820.0, 420245.0, 420830.0]</t>
-  </si>
-  <si>
-    <t>[310850.0, 311270.0, 312780.0, 312030.0, 313657.0, 312670.0]</t>
-  </si>
-  <si>
-    <t>[350920.0, 351630.0, 352850.0, 350900.0, 351640.0]</t>
-  </si>
-  <si>
-    <t>[313440.0, 316130.0, 312710.0, 313862.0, 311690.0, 315160.0, 317043.0, 312700.0, 313340.0, 315070.0, 311455.0]</t>
-  </si>
-  <si>
-    <t>[260100.0, 261510.0, 260750.0, 260880.0, 260240.0, 261010.0, 260370.0, 260380.0, 261030.0, 260650.0, 261320.0, 260050.0, 260825.0, 260830.0, 260320.0, 260330.0, 261230.0, 260210.0, 260470.0, 260600.0, 260860.0]</t>
-  </si>
-  <si>
-    <t>[510625.0, 510628.0, 510180.0, 510820.0, 510665.0, 510670.0, 510100.0, 510260.0, 510390.0, 510719.0]</t>
-  </si>
-  <si>
-    <t>[260900.0, 261380.0, 260070.0, 260550.0, 260360.0, 260780.0, 260620.0, 260460.0, 261530.0, 260765.0]</t>
-  </si>
-  <si>
-    <t>[316160.0, 312580.0, 316165.0, 316550.0, 317190.0, 316300.0, 316950.0, 312730.0, 314010.0, 312220.0, 313507.0, 310180.0, 316840.0, 312750.0, 312370.0, 314420.0, 312770.0, 317150.0, 311265.0, 316770.0, 315750.0, 313320.0, 311920.0, 312690.0]</t>
-  </si>
-  <si>
-    <t>[354880.0, 354410.0, 352940.0, 351380.0, 354870.0, 354330.0, 354780.0]</t>
-  </si>
-  <si>
-    <t>[420230.0, 420110.0, 420370.0, 420120.0, 421660.0, 421020.0, 421150.0, 421800.0, 421430.0, 420540.0, 421570.0, 421190.0, 421590.0, 420570.0, 420060.0, 421725.0, 420070.0, 421230.0, 420980.0, 420600.0, 420090.0, 421630.0]</t>
-  </si>
-  <si>
-    <t>[291200.0, 291077.0, 293000.0, 292105.0, 291340.0, 293260.0, 291733.0, 290710.0, 291740.0, 292640.0, 291875.0, 292020.0, 290500.0, 292680.0, 292180.0, 290520.0, 291170.0, 292450.0, 291940.0, 290660.0, 293105.0, 290420.0, 292340.0]</t>
-  </si>
-  <si>
-    <t>[315680.0, 312800.0, 316610.0, 312260.0, 314060.0, 315600.0, 311380.0, 312310.0, 317180.0]</t>
-  </si>
-  <si>
-    <t>[310950.0, 312870.0, 316390.0, 314410.0, 310410.0, 313690.0, 314300.0, 312830.0]</t>
-  </si>
-  <si>
-    <t>[350560.0, 355170.0, 354020.0, 351460.0, 353130.0, 354090.0, 352430.0, 351860.0, 353950.0]</t>
-  </si>
-  <si>
-    <t>[292320.0, 292225.0, 292160.0, 290475.0, 292370.0, 290450.0, 291410.0, 291320.0, 290270.0]</t>
-  </si>
-  <si>
-    <t>[170625.0, 172097.0, 170820.0, 170950.0, 170730.0, 171884.0, 170765.0, 171150.0, 171660.0, 171889.0, 170386.0, 170035.0, 172049.0, 172085.0, 170070.0, 171575.0, 170200.0, 172025.0]</t>
-  </si>
-  <si>
-    <t>[291360.0, 291490.0, 293250.0, 292805.0, 290630.0, 290225.0, 293270.0, 292090.0]</t>
-  </si>
-  <si>
-    <t>[211105.0, 210530.0, 210405.0, 210598.0, 210375.0, 210280.0, 211176.0, 210955.0, 211180.0, 210700.0, 210060.0, 210255.0, 210900.0, 210550.0, 210455.0, 210235.0]</t>
-  </si>
-  <si>
-    <t>[310880.0, 312250.0, 312930.0, 310050.0, 316260.0, 314435.0, 310630.0, 313610.0, 313130.0, 310925.0, 314995.0, 315895.0, 314170.0, 313115.0]</t>
-  </si>
-  <si>
-    <t>[291460.0, 291850.0, 290323.0, 291240.0, 291130.0, 290620.0, 292925.0, 290115.0, 290760.0, 291915.0, 291535.0, 292560.0, 290530.0, 292205.0, 291310.0, 293360.0, 293240.0, 291835.0, 290300.0]</t>
-  </si>
-  <si>
-    <t>[280290.0, 280100.0, 280390.0, 280230.0, 280680.0, 280520.0, 280140.0, 280370.0, 280050.0, 280500.0, 280600.0, 280410.0, 280700.0, 280445.0]</t>
-  </si>
-  <si>
-    <t>[293280.0, 290405.0, 291500.0, 290380.0, 291900.0, 291470.0, 292080.0, 292720.0, 290130.0, 291190.0, 291960.0, 291260.0, 293340.0, 292285.0]</t>
-  </si>
-  <si>
-    <t>[313280.0, 316480.0, 314370.0, 314750.0, 315720.0, 310540.0, 312590.0, 311535.0, 313170.0, 310770.0, 316050.0, 315800.0, 316190.0]</t>
-  </si>
-  <si>
-    <t>[290560.0, 291210.0, 291855.0, 291480.0, 290330.0, 291100.0, 291620.0, 292390.0, 290470.0, 290090.0, 292780.0, 290240.0, 291270.0, 292935.0, 291660.0, 291150.0, 291540.0, 291550.0, 293220.0, 292070.0, 293230.0, 290800.0]</t>
-  </si>
-  <si>
-    <t>[316320.0, 315100.0, 312740.0, 317220.0, 313990.0, 311720.0, 311850.0, 314730.0, 310890.0, 314040.0, 312110.0, 315090.0, 313240.0, 316540.0, 314910.0]</t>
-  </si>
-  <si>
-    <t>[311080.0, 312680.0, 316330.0, 313270.0, 315000.0, 314490.0]</t>
-  </si>
-  <si>
-    <t>[314315.0, 315217.0, 313330.0, 311700.0, 313400.0, 314140.0]</t>
-  </si>
-  <si>
-    <t>[211040.0, 210720.0, 210880.0, 211270.0, 210663.0, 210540.0, 210930.0, 210675.0, 210100.0, 210070.0, 211290.0, 211260.0, 210173.0, 210270.0]</t>
-  </si>
-  <si>
-    <t>[291680.0, 292000.0, 291970.0, 291580.0, 292270.0, 290480.0, 291090.0, 291710.0, 291350.0, 291640.0, 292540.0, 291230.0]</t>
-  </si>
-  <si>
-    <t>[350945.0, 352230.0, 355110.0, 355400.0, 351850.0, 350220.0, 351020.0, 351150.0, 355020.0, 354325.0, 354165.0, 351160.0, 350075.0]</t>
-  </si>
-  <si>
-    <t>[352320.0, 353282.0, 350535.0, 354280.0, 352265.0, 352170.0, 354350.0, 351760.0, 352240.0, 350800.0, 352215.0, 355385.0, 350715.0, 354300.0, 350270.0]</t>
-  </si>
-  <si>
-    <t>[313220.0, 313370.0, 315060.0, 313380.0]</t>
-  </si>
-  <si>
-    <t>[310980.0, 311110.0, 313420.0, 315980.0, 312910.0, 311180.0, 313140.0, 311580.0, 311260.0]</t>
-  </si>
-  <si>
-    <t>[292480.0, 293130.0, 292120.0, 291750.0, 292010.0, 292140.0, 293305.0, 293310.0, 293315.0, 293060.0, 292937.0, 292170.0, 290510.0, 292335.0, 292593.0, 292980.0, 290550.0, 293245.0, 290687.0]</t>
-  </si>
-  <si>
-    <t>[354720.0, 352480.0, 352965.0, 354025.0, 354570.0, 354765.0, 352910.0, 355695.0, 353520.0, 351420.0, 354900.0, 350260.0, 353590.0, 351385.0, 350395.0, 355580.0]</t>
-  </si>
-  <si>
-    <t>[313505.0, 314085.0, 313925.0, 313510.0, 314505.0, 312430.0, 317103.0, 314290.0, 314100.0, 315220.0, 316695.0, 315450.0, 311547.0, 312733.0, 314655.0]</t>
-  </si>
-  <si>
-    <t>[314915.0, 311783.0, 310825.0, 313520.0, 313210.0]</t>
-  </si>
-  <si>
-    <t>[352000.0, 352290.0, 350530.0, 350790.0, 350680.0, 352200.0, 350730.0, 355470.0, 352530.0, 351410.0, 352980.0, 350520.0]</t>
-  </si>
-  <si>
-    <t>[290310.0, 290950.0, 292490.0, 290060.0, 290195.0, 291870.0, 291760.0, 292790.0, 291510.0, 291000.0, 292280.0, 291390.0, 291520.0, 291905.0, 290370.0, 292040.0, 292050.0, 291670.0, 291800.0, 291290.0, 291420.0, 291430.0, 291690.0, 291570.0, 291830.0, 290430.0]</t>
-  </si>
-  <si>
-    <t>[352450.0, 355715.0, 350020.0, 353990.0, 353960.0, 355535.0, 355570.0, 353140.0, 353270.0, 352950.0, 352570.0]</t>
-  </si>
-  <si>
-    <t>[316100.0, 314470.0, 310600.0, 315570.0, 313620.0]</t>
-  </si>
-  <si>
-    <t>[313753.0, 313630.0, 310855.0]</t>
-  </si>
-  <si>
-    <t>[290720.0, 291840.0, 290990.0, 293200.0, 292600.0, 293077.0, 292440.0, 290682.0, 293020.0, 290590.0]</t>
-  </si>
-  <si>
-    <t>[314080.0, 312738.0, 315010.0, 311620.0, 311590.0, 313670.0, 316750.0, 310610.0, 315540.0, 315860.0, 312500.0, 311960.0]</t>
-  </si>
-  <si>
-    <t>[355650.0, 352520.0, 352590.0, 352400.0, 350960.0, 350840.0, 352730.0]</t>
-  </si>
-  <si>
-    <t>[120033.0, 120035.0, 120039.0, 120042.0, 120020.0, 120060.0, 120030.0]</t>
-  </si>
-  <si>
-    <t>[280740.0, 280580.0, 280710.0, 280550.0, 280620.0, 280350.0]</t>
-  </si>
-  <si>
-    <t>[150178.0, 150309.0, 150506.0, 150795.0, 150380.0, 150810.0]</t>
-  </si>
-  <si>
-    <t>[316040.0, 314890.0, 310420.0, 313720.0, 313530.0]</t>
-  </si>
-  <si>
-    <t>[350210.0, 351780.0, 353320.0, 352650.0, 353740.0, 352044.0, 352300.0, 353010.0, 355255.0, 353210.0, 351100.0, 355230.0]</t>
-  </si>
-  <si>
-    <t>[420610.0, 421700.0, 420280.0, 421545.0, 420395.0, 420620.0, 420940.0, 421560.0, 421870.0, 421840.0, 420720.0, 420880.0, 421490.0, 421710.0, 421265.0, 420150.0, 421240.0, 420730.0]</t>
-  </si>
-  <si>
-    <t>[311460.0, 313450.0, 313870.0, 314460.0, 313040.0, 315470.0, 314990.0, 313430.0, 313080.0, 313820.0]</t>
-  </si>
-  <si>
-    <t>[315840.0, 312290.0, 310440.0, 313800.0, 311530.0, 313260.0, 314670.0, 313840.0, 315410.0, 310460.0]</t>
-  </si>
-  <si>
-    <t>[310720.0, 313860.0, 310680.0, 315590.0, 310280.0, 314540.0, 315727.0, 313850.0, 310360.0, 314780.0, 315930.0, 314940.0, 310750.0]</t>
-  </si>
-  <si>
-    <t>[351240.0, 352690.0, 351515.0, 352140.0]</t>
-  </si>
-  <si>
-    <t>[260490.0, 260890.0, 260270.0, 260910.0, 260400.0, 261550.0, 261050.0, 260540.0, 260415.0, 261060.0, 261450.0, 260810.0, 260950.0, 261210.0, 260970.0, 260845.0, 260850.0, 261618.0, 260220.0, 261630.0]</t>
-  </si>
-  <si>
-    <t>[350880.0, 352710.0, 355590.0, 351720.0, 354160.0, 351700.0, 354010.0, 354460.0]</t>
-  </si>
-  <si>
-    <t>[352040.0, 351050.0, 355540.0, 355070.0]</t>
-  </si>
-  <si>
-    <t>[110080.0, 110020.0, 110033.0, 110010.0, 110110.0]</t>
-  </si>
-  <si>
-    <t>[351300.0, 351500.0, 352620.0, 355280.0, 354995.0, 351510.0, 352220.0, 355645.0]</t>
-  </si>
-  <si>
-    <t>[130115.0, 130310.0, 130185.0, 130380.0, 130030.0, 130255.0, 130353.0, 130260.0, 130356.0, 130040.0, 130360.0, 130110.0]</t>
-  </si>
-  <si>
-    <t>[313930.0, 314225.0, 316245.0, 314270.0, 313695.0]</t>
-  </si>
-  <si>
-    <t>[316805.0, 313867.0, 315790.0, 310030.0, 315415.0, 313120.0, 314400.0, 312352.0, 313770.0, 311600.0, 315190.0, 311740.0, 310205.0, 314053.0, 316360.0, 313940.0, 315350.0, 316760.0, 313950.0, 316255.0, 314090.0, 315890.0, 311290.0]</t>
-  </si>
-  <si>
-    <t>[316257.0, 314467.0, 314150.0, 313960.0, 316105.0, 311570.0, 312210.0, 313180.0]</t>
-  </si>
-  <si>
-    <t>[355330.0, 354630.0, 354910.0, 350030.0, 350040.0, 355640.0, 354810.0, 351518.0]</t>
-  </si>
-  <si>
-    <t>[150630.0, 150790.0, 150250.0, 150570.0, 150030.0, 150640.0, 150770.0, 150200.0, 150490.0]</t>
-  </si>
-  <si>
-    <t>[150180.0, 150310.0, 150280.0, 150450.0, 150580.0, 150070.0, 150110.0]</t>
-  </si>
-  <si>
-    <t>[353410.0, 352900.0, 350980.0, 352780.0, 354200.0, 353450.0, 351660.0, 351670.0, 350140.0, 351810.0, 352580.0, 350150.0, 355660.0, 351565.0, 354000.0, 353370.0, 355550.0, 351470.0, 351730.0]</t>
-  </si>
-  <si>
-    <t>[420360.0, 421003.0, 421915.0, 421917.0, 420900.0, 420005.0, 420390.0, 420520.0, 420400.0, 420920.0, 421180.0, 420670.0, 420287.0, 420415.0, 420680.0, 420040.0, 421850.0, 421985.0, 421105.0, 420860.0]</t>
-  </si>
-  <si>
-    <t>[320130.0, 320520.0, 320010.0, 320270.0, 320530.0, 320250.0, 320290.0, 320170.0, 320313.0, 320316.0, 320060.0, 320190.0, 320450.0, 320455.0, 320460.0, 320334.0, 320220.0, 320240.0, 320115.0, 320500.0, 320245.0, 320506.0, 320510.0]</t>
-  </si>
-  <si>
-    <t>[150080.0, 150150.0, 150442.0, 150635.0, 150140.0]</t>
-  </si>
-  <si>
-    <t>[330250.0, 330285.0, 330510.0, 330414.0, 330320.0, 330350.0, 330227.0, 330455.0, 330200.0, 330170.0, 330555.0, 330045.0]</t>
-  </si>
-  <si>
-    <t>[150275.0, 150020.0, 150820.0, 150700.0, 150190.0, 150800.0, 150260.0, 150710.0, 150650.0]</t>
-  </si>
-  <si>
-    <t>[330560.0, 330490.0, 330270.0, 330190.0, 330575.0, 330330.0, 330430.0]</t>
-  </si>
-  <si>
-    <t>[150660.0, 150405.0, 150410.0, 150796.0, 150290.0, 150550.0, 150812.0, 150430.0, 150307.0, 150440.0, 150320.0, 150720.0, 150340.0, 150345.0, 150350.0, 150095.0, 150740.0, 150230.0, 150746.0, 150495.0, 150240.0, 150760.0]</t>
-  </si>
-  <si>
-    <t>[311650.0, 313680.0, 313200.0, 314200.0, 314330.0, 312735.0]</t>
-  </si>
-  <si>
-    <t>[314210.0, 314820.0, 310310.0, 312490.0, 316140.0, 314220.0, 317140.0, 310550.0, 314390.0, 316443.0, 315645.0]</t>
-  </si>
-  <si>
-    <t>[130400.0, 130440.0, 130190.0, 130200.0, 130395.0, 130430.0]</t>
-  </si>
-  <si>
-    <t>[510020.0, 510310.0, 510185.0, 510718.0, 510385.0, 510706.0, 510617.0, 510270.0]</t>
-  </si>
-  <si>
-    <t>[171488.0, 170210.0, 171395.0, 170307.0, 170215.0, 171720.0, 171630.0, 171886.0, 170384.0, 172208.0, 172210.0, 170770.0, 170388.0, 170900.0, 170130.0, 170650.0, 170300.0]</t>
-  </si>
-  <si>
-    <t>[510787.0, 510885.0, 510726.0, 510345.0, 510795.0, 510130.0, 510263.0, 510170.0, 510685.0, 510623.0]</t>
-  </si>
-  <si>
-    <t>[330400.0, 330630.0, 330440.0, 330411.0, 330412.0, 330030.0, 330225.0, 330450.0, 330610.0, 330420.0, 330040.0, 330395.0]</t>
-  </si>
-  <si>
-    <t>[420290.0, 420515.0, 421510.0, 421320.0, 420170.0, 421820.0, 420590.0, 420270.0, 420240.0, 420750.0, 420630.0, 420220.0, 420125.0, 421470.0]</t>
-  </si>
-  <si>
-    <t>[314430.0, 311370.0, 316670.0]</t>
-  </si>
-  <si>
-    <t>[420130.0, 420580.0, 420845.0, 420205.0, 420910.0, 421620.0]</t>
-  </si>
-  <si>
-    <t>[521350.0, 520490.0, 520530.0, 522108.0, 520830.0]</t>
-  </si>
-  <si>
-    <t>[520670.0, 521830.0, 520396.0, 520940.0, 520080.0, 521490.0, 522068.0, 522070.0, 521270.0, 521980.0, 520990.0]</t>
-  </si>
-  <si>
-    <t>[330210.0, 330115.0, 330470.0, 330310.0, 330090.0, 330410.0, 330060.0, 330220.0, 330513.0, 330230.0, 330615.0, 330300.0, 330205.0, 330015.0]</t>
-  </si>
-  <si>
-    <t>[510337.0, 510285.0, 510190.0, 510515.0, 510517.0, 510325.0, 510140.0]</t>
-  </si>
-  <si>
-    <t>[521377.0, 521410.0, 522145.0, 522020.0, 520357.0, 521960.0, 521800.0, 520810.0, 520750.0, 520465.0, 521525.0, 521308.0, 521405.0]</t>
-  </si>
-  <si>
-    <t>[330240.0, 330500.0, 330475.0, 330093.0, 330415.0, 330480.0, 330100.0, 330140.0]</t>
-  </si>
-  <si>
-    <t>[351200.0, 352420.0, 351210.0, 350090.0, 353390.0, 351790.0, 350930.0, 350550.0, 355190.0, 351740.0]</t>
-  </si>
-  <si>
-    <t>[510785.0, 510530.0, 510788.0, 510631.0, 510035.0]</t>
-  </si>
-  <si>
-    <t>[510880.0, 510320.0, 510455.0, 510619.0, 510621.0, 510558.0]</t>
-  </si>
-  <si>
-    <t>[352930.0, 351010.0, 351400.0, 355370.0, 354650.0]</t>
-  </si>
-  <si>
-    <t>[280450.0, 280260.0, 280420.0, 280540.0, 280240.0, 280560.0, 280310.0, 280120.0, 280220.0]</t>
-  </si>
-  <si>
-    <t>[280480.0, 280610.0, 280130.0, 280330.0, 280460.0, 280720.0, 280400.0, 280530.0, 280660.0, 280150.0, 280250.0, 280190.0]</t>
-  </si>
-  <si>
-    <t>[421507.0, 421775.0, 421140.0, 421145.0, 420895.0, 421290.0, 421420.0, 420785.0, 420665.0, 420410.0, 420543.0, 421569.0, 421315.0, 420420.0, 420165.0, 421187.0, 420050.0, 420435.0, 420310.0, 420055.0, 420440.0, 421210.0, 421600.0, 421755.0, 420470.0, 420475.0, 421885.0]</t>
-  </si>
-  <si>
-    <t>[521030.0, 521020.0, 521160.0, 521720.0, 520170.0, 520235.0, 520710.0, 521200.0, 521520.0, 520340.0, 520310.0, 520760.0, 521370.0, 521340.0, 521565.0, 520090.0]</t>
-  </si>
-  <si>
-    <t>[521570.0, 520260.0, 520420.0, 522150.0, 521640.0, 520393.0, 520780.0, 521900.0, 520015.0, 522005.0, 521590.0, 520570.0, 522010.0]</t>
-  </si>
-  <si>
-    <t>[510720.0, 510562.0, 510343.0, 510250.0, 510125.0, 510450.0, 510395.0, 510710.0, 510775.0, 510682.0, 510523.0, 510715.0]</t>
-  </si>
-  <si>
-    <t>[314560.0, 311400.0, 314770.0, 315990.0, 316120.0, 311450.0]</t>
-  </si>
-  <si>
-    <t>[261255.0, 260200.0, 260110.0, 261040.0, 260530.0, 261430.0, 260630.0, 261560.0, 260730.0, 261245.0, 260990.0]</t>
-  </si>
-  <si>
-    <t>[355460.0, 353380.0, 350630.0, 351015.0, 355720.0, 355050.0, 354540.0, 351950.0, 354640.0, 354320.0, 352090.0, 353470.0, 351519.0]</t>
-  </si>
-  <si>
-    <t>[314000.0, 314610.0, 313190.0]</t>
-  </si>
-  <si>
-    <t>[311545.0, 313230.0, 311300.0, 314630.0]</t>
-  </si>
-  <si>
-    <t>[260480.0, 260870.0, 261000.0, 261650.0, 261140.0, 261150.0, 260520.0, 261290.0, 261420.0, 260140.0, 260150.0, 260920.0, 260795.0, 261180.0, 260420.0, 261190.0, 260040.0, 260820.0, 261340.0, 261485.0, 260590.0, 260090.0]</t>
-  </si>
-  <si>
-    <t>[315140.0, 313830.0, 311760.0, 314580.0, 316310.0, 314710.0, 314520.0, 313020.0]</t>
-  </si>
-  <si>
-    <t>[316294.0, 314790.0, 310760.0, 310190.0, 314510.0, 311440.0, 312630.0, 316220.0, 313375.0]</t>
-  </si>
-  <si>
-    <t>[312070.0, 316680.0, 316170.0, 317100.0, 315340.0, 313710.0, 314800.0, 317075.0, 313750.0, 312890.0, 312860.0]</t>
-  </si>
-  <si>
-    <t>[312480.0, 314310.0, 313160.0, 310010.0, 311930.0, 312790.0, 315640.0, 314810.0, 312350.0]</t>
-  </si>
-  <si>
-    <t>[291810.0, 290020.0, 292420.0, 292710.0, 291140.0, 292400.0, 290770.0, 291990.0, 292760.0]</t>
-  </si>
-  <si>
-    <t>[312235.0, 310100.0, 312245.0, 314870.0, 310270.0]</t>
-  </si>
-  <si>
-    <t>[210400.0, 210594.0, 210596.0, 210820.0, 210600.0, 210570.0, 210890.0, 210193.0, 210580.0, 211223.0, 210520.0, 211163.0, 211167.0]</t>
-  </si>
-  <si>
-    <t>[260515.0, 260875.0, 260300.0, 261260.0, 260980.0, 260020.0, 261110.0]</t>
-  </si>
-  <si>
-    <t>[311205.0, 314860.0, 316280.0, 312695.0, 314840.0, 316410.0, 316350.0]</t>
-  </si>
-  <si>
-    <t>[210370.0, 210083.0, 210980.0, 210310.0, 210312.0, 210825.0, 211178.0, 211240.0, 210860.0, 211245.0, 210190.0, 210927.0, 210130.0, 210840.0, 210680.0, 210905.0, 210490.0]</t>
-  </si>
-  <si>
-    <t>[354400.0, 351040.0, 353090.0, 354210.0, 351170.0, 351490.0, 355040.0, 354700.0, 350060.0, 353870.0, 354515.0]</t>
-  </si>
-  <si>
-    <t>[312960.0, 315213.0, 315120.0, 315760.0, 313810.0, 317080.0, 310940.0]</t>
-  </si>
-  <si>
-    <t>[521730.0, 520580.0, 520485.0, 520551.0, 522119.0, 520840.0, 520010.0, 520110.0, 520815.0, 520030.0]</t>
-  </si>
-  <si>
-    <t>[317060.0, 315050.0, 312810.0, 316430.0, 315150.0, 311280.0, 312340.0]</t>
-  </si>
-  <si>
-    <t>[421500.0, 421220.0, 421030.0, 421830.0, 420330.0, 420810.0, 421580.0, 421360.0, 421010.0, 420213.0, 420790.0, 421110.0, 420380.0]</t>
-  </si>
-  <si>
-    <t>[220669.0, 220770.0, 220200.0, 220265.0, 220270.0, 220272.0, 220208.0, 220465.0, 220570.0, 220253.0, 220191.0]</t>
-  </si>
-  <si>
-    <t>[352640.0, 354050.0, 350690.0, 355010.0, 350750.0, 355465.0, 353610.0, 351230.0, 350230.0, 350360.0, 354105.0, 353750.0, 352350.0]</t>
-  </si>
-  <si>
-    <t>[354425.0, 353020.0, 355430.0, 351535.0]</t>
-  </si>
-  <si>
-    <t>[315400.0, 315020.0, 316556.0, 310040.0, 310570.0, 316340.0, 315210.0, 312270.0, 313550.0, 316630.0, 310230.0, 314585.0, 315740.0, 315490.0, 312170.0, 310250.0, 315500.0, 316010.0, 316400.0, 312820.0, 317050.0]</t>
-  </si>
-  <si>
-    <t>[291072.0, 292770.0, 290340.0, 291465.0, 291530.0, 291180.0, 291630.0, 292530.0]</t>
-  </si>
-  <si>
-    <t>[312450.0, 310790.0, 311050.0, 314380.0, 316557.0, 313360.0, 313490.0, 311060.0, 316440.0, 316580.0, 310830.0, 316980.0, 311990.0, 315960.0, 310970.0, 313150.0, 312510.0, 311360.0, 316740.0, 316230.0, 314440.0, 312920.0, 313060.0, 311780.0, 314340.0, 314600.0, 316905.0, 316910.0, 311790.0, 315250.0, 312440.0, 310910.0]</t>
-  </si>
-  <si>
-    <t>[315180.0, 315920.0, 310260.0, 311030.0, 310140.0, 312990.0]</t>
-  </si>
-  <si>
-    <t>[210560.0, 210275.0, 211174.0, 210462.0, 210440.0, 210470.0, 210380.0, 210450.0, 210420.0, 211125.0, 211030.0, 210910.0, 211070.0, 210460.0, 211230.0, 210975.0]</t>
-  </si>
-  <si>
-    <t>[280640.0, 280160.0, 280070.0, 280730.0, 280010.0, 280490.0, 280110.0, 280270.0, 280430.0, 280690.0, 280340.0, 280020.0, 280470.0, 280440.0, 280570.0, 280380.0]</t>
-  </si>
-  <si>
-    <t>[260610.0, 261640.0, 260105.0, 261130.0, 260760.0, 260005.0, 260775.0, 261160.0, 260790.0, 260545.0, 260290.0, 260680.0, 260940.0, 261070.0, 260440.0, 260960.0, 260450.0, 260720.0, 260345.0, 261370.0]</t>
-  </si>
-  <si>
-    <t>[130180.0, 130150.0, 130195.0, 130100.0, 130165.0, 130140.0]</t>
-  </si>
-  <si>
-    <t>[130240.0, 130410.0, 130090.0, 130350.0, 130070.0]</t>
-  </si>
-  <si>
-    <t>[431120.0, 432149.0, 431912.0, 431402.0, 431532.0, 430637.0, 430010.0, 431550.0, 432065.0, 431940.0, 431690.0, 431053.0, 430670.0, 431310.0, 430800.0, 431447.0, 431960.0, 432345.0, 432220.0, 431843.0, 431075.0, 430840.0]</t>
-  </si>
-  <si>
-    <t>[430465.0, 431810.0, 431110.0, 431303.0, 431113.0, 431210.0, 431980.0, 432237.0, 431055.0, 430290.0, 431740.0]</t>
-  </si>
-  <si>
-    <t>[431171.0, 431175.0, 431640.0, 431530.0, 430187.0, 432240.0, 431697.0, 431060.0, 431830.0, 430040.0, 431710.0]</t>
-  </si>
-  <si>
-    <t>[431173.0, 432166.0, 431177.0, 431244.0, 430655.0, 432143.0, 431065.0, 432150.0, 432183.0, 430105.0, 432380.0, 430463.0]</t>
-  </si>
-  <si>
-    <t>[432160.0, 430467.0, 431365.0, 432135.0, 430471.0, 431760.0, 430545.0, 431250.0, 430163.0, 431350.0, 431033.0]</t>
-  </si>
-  <si>
-    <t>[430360.0, 431010.0, 432170.0, 431820.0, 431405.0, 431600.0, 431575.0, 432120.0]</t>
-  </si>
-  <si>
-    <t>[430087.0, 430760.0, 431080.0, 431306.0, 431848.0, 431340.0, 431247.0, 430640.0, 431514.0, 431695.0, 430390.0, 431990.0, 431480.0, 431162.0, 431870.0]</t>
-  </si>
-  <si>
-    <t>[432000.0, 432225.0, 431650.0, 430468.0, 431240.0, 431337.0, 432200.0, 430955.0, 431403.0, 431179.0, 431950.0, 430770.0, 431861.0, 430165.0, 432085.0, 430265.0, 430460.0, 431935.0]</t>
-  </si>
-  <si>
-    <t>[430085.0, 430605.0, 430350.0, 430110.0, 430880.0, 432035.0, 430517.0, 432055.0, 430650.0, 430270.0, 430535.0, 430544.0, 430930.0, 430676.0, 431198.0, 430175.0, 431840.0, 432110.0, 430190.0, 431225.0]</t>
-  </si>
-  <si>
-    <t>[431490.0, 430310.0, 430920.0, 432300.0, 430060.0, 430905.0]</t>
-  </si>
-  <si>
-    <t>[431750.0, 431630.0, 430865.0, 431890.0, 431510.0, 431770.0, 431647.0, 430250.0, 431915.0, 430635.0, 431920.0, 431800.0, 432057.0, 430520.0, 430783.0, 431937.0, 431455.0, 430693.0, 430950.0, 432234.0, 431595.0, 431217.0, 432375.0, 430330.0]</t>
-  </si>
-  <si>
-    <t>[430560.0, 431645.0, 430222.0, 431535.0, 431087.0, 430223.0, 430610.0, 431670.0, 431000.0, 431643.0, 430845.0, 432030.0]</t>
-  </si>
-  <si>
-    <t>[430600.0, 431115.0, 432023.0, 431390.0, 430500.0, 431780.0, 431910.0, 431020.0, 430258.0, 430400.0, 431041.0, 430020.0, 431430.0, 430150.0, 430540.0, 431973.0, 431333.0, 430570.0, 430970.0, 430587.0]</t>
-  </si>
-  <si>
-    <t>[430220.0, 431500.0, 431505.0, 431507.0, 432032.0, 430370.0, 431790.0, 432180.0, 430900.0, 431930.0, 431040.0, 431301.0, 430030.0, 430673.0, 432210.0, 430045.0, 430430.0, 432230.0, 431720.0, 431849.0, 431342.0, 430960.0]</t>
-  </si>
-  <si>
-    <t>[430850.0, 432132.0, 430340.0, 430730.0, 432140.0, 430607.0, 432147.0, 431380.0, 432020.0, 430745.0, 430237.0, 430632.0, 432310.0, 431160.0, 432190.0, 431050.0, 431445.0, 431449.0, 432350.0, 430050.0, 431590.0, 430185.0, 431470.0, 430064.0, 431344.0, 432370.0]</t>
-  </si>
-  <si>
-    <t>[430720.0, 430090.0, 430613.0, 430870.0, 430485.0, 432290.0, 430755.0, 432163.0, 431270.0, 430890.0, 431531.0, 430380.0, 430511.0, 431413.0, 432060.0, 431555.0, 431046.0, 430537.0, 430155.0, 430805.0, 431190.0, 430170.0, 431070.0, 431200.0, 431970.0, 430695.0, 430697.0, 430825.0, 430700.0, 430192.0, 431090.0, 431478.0, 430205.0]</t>
-  </si>
-  <si>
-    <t>[431235.0, 430597.0, 430470.0, 431755.0, 430355.0, 431127.0, 430490.0, 431262.0, 431775.0, 431265.0, 431267.0, 430885.0, 430630.0, 432040.0, 431275.0, 432050.0, 431410.0, 431805.0, 432320.0, 431180.0, 432340.0, 430550.0, 430047.0, 431213.0, 430705.0, 431477.0, 430585.0, 432255.0]</t>
-  </si>
-  <si>
-    <t>[431360.0, 430980.0, 430990.0, 431130.0, 430495.0, 431660.0, 431795.0, 430005.0, 431673.0, 431170.0, 432335.0, 432090.0, 432218.0, 431842.0, 430180.0, 430320.0, 430066.0, 431860.0, 431220.0, 430462.0]</t>
-  </si>
-  <si>
-    <t>[432100.0, 430055.0, 431242.0, 430410.0, 430830.0, 432080.0, 431057.0, 432146.0, 430995.0, 431125.0, 432215.0, 430200.0, 430140.0, 430750.0]</t>
-  </si>
-  <si>
-    <t>[431620.0, 430590.0, 430215.0, 432010.0, 431370.0, 431642.0, 431142.0, 430642.0, 430515.0, 430260.0, 431540.0, 432185.0, 431295.0, 431936.0, 430912.0, 430530.0, 432195.0, 430692.0, 431845.0, 431085.0, 431346.0, 430195.0, 430580.0, 431349.0, 431610.0, 431230.0]</t>
-  </si>
-  <si>
-    <t>[430466.0, 431880.0, 431245.0, 430107.0, 430512.0, 430130.0, 431417.0, 431420.0, 431560.0, 430543.0, 431440.0, 431700.0, 431450.0, 431460.0, 432232.0, 431850.0, 430063.0, 431730.0, 430450.0, 430710.0, 431100.0]</t>
-  </si>
-  <si>
-    <t>[430435.0, 430660.0, 431150.0, 430160.0, 430003.0, 430965.0]</t>
-  </si>
-  <si>
-    <t>[430440.0, 430510.0, 431442.0, 431320.0, 431164.0, 430910.0]</t>
-  </si>
-  <si>
-    <t>[431237.0, 431112.0, 430740.0, 431446.0, 431862.0, 430230.0, 432250.0, 431261.0, 430367.0]</t>
-  </si>
-  <si>
-    <t>[430593.0, 430210.0, 430595.0, 431238.0, 430860.0, 430480.0, 430225.0, 432280.0, 431517.0, 431400.0, 431280.0, 431290.0, 430786.0, 432330.0, 430925.0, 430940.0, 431454.0, 431330.0, 431844.0, 432360.0, 432235.0, 431725.0]</t>
-  </si>
-  <si>
-    <t>[430080.0, 431043.0, 430820.0, 430790.0, 431975.0, 431335.0, 430057.0, 431308.0, 430810.0, 430235.0, 431900.0, 432254.0]</t>
-  </si>
-  <si>
-    <t>[430690.0, 432070.0, 430120.0, 430280.0, 431339.0, 431406.0, 430513.0, 431123.0, 432026.0, 430300.0, 430781.0, 430975.0]</t>
-  </si>
-  <si>
-    <t>[431680.0, 432067.0, 432260.0, 430915.0, 431395.0, 430957.0, 432270.0, 431407.0, 431215.0, 431570.0, 430420.0, 432252.0, 432253.0]</t>
-  </si>
-  <si>
-    <t>[430469.0, 430100.0, 431513.0, 431515.0, 430620.0, 432285.0, 431260.0, 431520.0, 432162.0, 431140.0, 430245.0, 432045.0, 430645.0, 431030.0, 431545.0, 431675.0, 431300.0, 430675.0, 430680.0, 431580.0, 431971.0, 431205.0, 431846.0, 430070.0, 430583.0, 430843.0, 430461.0]</t>
-  </si>
-  <si>
-    <t>[430240.0, 430780.0, 432130.0, 430807.0, 432145.0, 431475.0, 431415.0, 432377.0, 431036.0, 430558.0]</t>
-  </si>
-  <si>
-    <t>[354580.0, 353180.0, 351905.0, 351907.0, 355620.0, 355240.0, 350380.0, 353710.0, 351280.0, 353200.0, 352050.0, 353340.0, 350160.0, 352340.0, 352470.0, 355670.0, 350950.0, 354800.0, 353650.0]</t>
-  </si>
-  <si>
-    <t>[311840.0, 312737.0, 313410.0, 315430.0, 310220.0, 315950.0, 312083.0, 310110.0]</t>
-  </si>
-  <si>
-    <t>[292290.0, 291075.0, 290790.0, 290920.0, 292650.0, 290160.0, 291185.0, 292305.0, 290035.0, 293076.0, 292660.0, 292310.0, 290265.0, 290780.0, 292380.0]</t>
-  </si>
-  <si>
-    <t>[150560.0, 150690.0, 150500.0, 150090.0, 150540.0, 150220.0, 150830.0, 150160.0, 150610.0, 150611.0, 150803.0, 150195.0, 150170.0, 150747.0, 150620.0, 150655.0]</t>
-  </si>
-  <si>
-    <t>[351270.0, 352360.0, 352110.0, 354670.0, 354390.0, 350200.0]</t>
-  </si>
-  <si>
-    <t>[130080.0, 130330.0, 130014.0, 130170.0, 130270.0]</t>
-  </si>
-  <si>
-    <t>[130083.0, 130120.0, 130250.0, 130063.0, 130320.0, 130130.0, 130008.0, 130010.0]</t>
-  </si>
-  <si>
-    <t>[355360.0, 355080.0, 351080.0, 350870.0, 354970.0, 353050.0, 352380.0, 351390.0]</t>
-  </si>
-  <si>
-    <t>[520960.0, 520929.0, 521120.0, 520250.0, 521925.0, 521220.0, 521483.0, 521100.0, 521390.0, 521295.0, 521040.0, 520753.0, 520085.0, 520215.0, 521400.0, 520890.0, 520380.0]</t>
-  </si>
-  <si>
-    <t>[210500.0, 210920.0, 211020.0, 210125.0, 210510.0, 210960.0, 211027.0, 210710.0, 210170.0, 210940.0, 210237.0, 210110.0]</t>
-  </si>
-  <si>
-    <t>[353440.0, 350570.0, 354730.0, 351060.0, 352500.0, 353910.0, 352250.0]</t>
-  </si>
-  <si>
-    <t>[260160.0, 260930.0, 261220.0, 261610.0, 260430.0, 261520.0, 261400.0]</t>
-  </si>
-  <si>
-    <t>[292740.0, 293320.0, 292975.0, 291920.0, 292950.0, 292920.0, 290650.0, 291610.0, 292860.0, 291992.0]</t>
-  </si>
-  <si>
-    <t>[355490.0, 354660.0, 353284.0, 354610.0, 354450.0, 354740.0]</t>
-  </si>
-  <si>
-    <t>[210465.0, 210850.0, 210690.0, 210177.0, 211172.0, 210200.0, 210990.0, 210515.0, 210870.0, 211000.0, 211227.0, 211102.0, 210047.0]</t>
-  </si>
-  <si>
-    <t>[293030.0, 292905.0, 292810.0, 291735.0, 290610.0, 293075.0, 290930.0, 292820.0, 290390.0, 293015.0, 290810.0, 290910.0]</t>
-  </si>
-  <si>
-    <t>[316450.0, 315820.0, 310060.0, 313655.0]</t>
-  </si>
-  <si>
-    <t>[292870.0, 290830.0, 292240.0, 292250.0, 292130.0, 291880.0, 290730.0, 292910.0, 290100.0, 290230.0, 291780.0, 293317.0, 292940.0, 291020.0, 291030.0, 293210.0, 292575.0, 291685.0, 291820.0, 292850.0, 292730.0, 292220.0]</t>
-  </si>
-  <si>
-    <t>[314570.0, 310330.0, 316070.0]</t>
-  </si>
-  <si>
-    <t>[290400.0, 292990.0, 291300.0, 291930.0, 292350.0, 292430.0, 292303.0, 291440.0, 293080.0, 290010.0, 292190.0]</t>
-  </si>
-  <si>
-    <t>[290180.0, 290600.0, 292460.0, 292525.0, 291085.0, 293010.0, 291700.0, 290135.0, 291770.0]</t>
-  </si>
-  <si>
-    <t>[421505.0, 421890.0, 420417.0, 420260.0, 420325.0, 420100.0, 421895.0, 420930.0, 420455.0, 421189.0, 421680.0, 421330.0, 421650.0, 420340.0, 420243.0, 421205.0, 421175.0, 420250.0]</t>
-  </si>
-  <si>
-    <t>[261570.0, 260740.0, 261350.0, 260392.0, 261390.0, 260560.0, 260180.0, 260340.0, 260570.0, 261247.0]</t>
-  </si>
-  <si>
-    <t>[220192.0, 221060.0, 220070.0, 220455.0, 221000.0, 220553.0, 221035.0, 220556.0, 220335.0, 221135.0, 220211.0, 220245.0, 220375.0, 220345.0, 220250.0, 220955.0, 220285.0, 220535.0]</t>
-  </si>
-  <si>
-    <t>[521280.0, 520552.0, 521487.0, 522160.0, 520082.0, 521460.0, 520980.0, 520470.0, 520055.0]</t>
-  </si>
-  <si>
-    <t>[330080.0, 330530.0, 330050.0, 330340.0, 330245.0, 330150.0, 330110.0, 330120.0, 330185.0, 330570.0, 330160.0, 330515.0, 330580.0, 330390.0, 330460.0, 330590.0]</t>
-  </si>
-  <si>
-    <t>[292610.0, 290327.0, 290840.0, 293150.0, 292895.0, 290210.0, 292265.0, 293300.0, 292150.0, 290360.0, 293050.0, 292800.0, 290040.0, 291910.0, 293190.0, 292580.0, 292590.0, 290680.0, 291070.0]</t>
-  </si>
-  <si>
-    <t>[310240.0, 311750.0, 316710.0, 316650.0, 316020.0]</t>
-  </si>
-  <si>
-    <t>[310020.0, 311560.0, 313100.0, 314640.0, 312720.0, 310700.0, 310320.0, 310960.0, 316720.0, 315200.0, 312640.0, 314690.0, 315850.0, 310990.0, 314960.0, 311890.0, 311250.0, 315360.0, 313570.0, 310500.0, 315370.0, 314350.0, 313970.0, 314740.0]</t>
-  </si>
-  <si>
-    <t>[352390.0, 354060.0, 355220.0, 355350.0, 350115.0, 351030.0, 350275.0, 352840.0, 352585.0, 350290.0, 354520.0, 354530.0, 351970.0, 352100.0, 350700.0, 353780.0, 355700.0, 355060.0, 355450.0, 353790.0]</t>
-  </si>
-  <si>
-    <t>[170240.0, 170560.0, 171620.0, 171525.0, 171780.0, 170700.0, 171215.0, 171800.0, 171515.0, 170040.0, 171865.0, 172090.0, 170555.0, 172093.0, 170270.0]</t>
-  </si>
-  <si>
-    <t>[521225.0, 521130.0, 522155.0, 521930.0, 520013.0, 521880.0, 520410.0, 520430.0, 520145.0, 522040.0, 521971.0, 521300.0, 521805.0, 521080.0, 520505.0, 521850.0, 521630.0, 521375.0]</t>
-  </si>
-  <si>
-    <t>[522050.0, 520547.0, 521190.0, 521645.0, 521810.0, 521940.0, 520725.0, 520150.0, 520440.0, 521310.0]</t>
-  </si>
-  <si>
-    <t>[510336.0, 510500.0, 510757.0, 510380.0, 510330.0, 510675.0, 510835.0, 510550.0, 510618.0, 510268.0]</t>
-  </si>
-  <si>
-    <t>[320260.0, 320265.0, 320140.0, 320020.0, 320280.0, 320030.0, 320420.0, 320040.0, 320300.0, 320430.0, 320050.0, 320180.0, 320310.0, 320440.0, 320070.0, 320200.0, 320332.0, 320340.0, 320480.0, 320230.0, 320110.0, 320370.0, 320503.0, 320120.0, 320380.0, 320255.0]</t>
-  </si>
-  <si>
-    <t>[521600.0, 520993.0, 521380.0, 520390.0, 520425.0, 520910.0, 520050.0, 520915.0, 520020.0, 521210.0, 520350.0, 521150.0]</t>
-  </si>
-  <si>
-    <t>[140028.0, 140047.0, 140050.0, 140020.0, 140023.0, 140060.0]</t>
-  </si>
-  <si>
-    <t>[355680.0, 355365.0, 355690.0, 355310.0, 355440.0, 350610.0, 355320.0, 353150.0]</t>
-  </si>
-  <si>
-    <t>[510729.0, 510480.0, 510740.0, 510360.0, 510630.0, 510120.0, 510760.0, 510637.0, 510520.0, 510779.0, 510267.0, 510030.0, 510420.0, 510040.0, 510810.0, 510060.0, 510700.0, 510704.0, 510460.0]</t>
-  </si>
-  <si>
-    <t>[315970.0, 311430.0, 314120.0, 310380.0, 316210.0, 316890.0, 315550.0]</t>
-  </si>
-  <si>
-    <t>[353280.0, 351750.0, 353030.0, 355340.0, 353420.0, 350480.0, 353040.0, 353300.0, 353660.0, 351130.0, 354080.0, 354980.0, 351940.0, 353500.0, 353250.0, 355560.0, 351980.0, 352115.0, 353400.0, 350460.0]</t>
-  </si>
-  <si>
-    <t>[311520.0, 311970.0, 315270.0, 313000.0, 315610.0, 313740.0, 312300.0, 310800.0, 316880.0, 316530.0, 314450.0, 316500.0, 315733.0, 315030.0, 313910.0, 316250.0, 315420.0, 310590.0]</t>
-  </si>
-  <si>
-    <t>[310690.0, 316290.0, 312130.0, 314020.0, 314950.0, 315620.0, 316560.0, 312850.0, 313980.0]</t>
-  </si>
-  <si>
-    <t>[210592.0, 210180.0, 210790.0, 211110.0, 210150.0, 210730.0, 210350.0, 210670.0, 210800.0, 210545.0, 210770.0, 210230.0, 211190.0, 211065.0, 211195.0]</t>
-  </si>
-  <si>
-    <t>[314760.0, 312080.0, 316700.0, 313780.0, 314550.0, 311480.0, 316490.0, 314190.0, 316370.0, 313300.0, 312280.0, 311770.0, 310490.0, 313310.0, 316640.0, 310120.0, 316780.0, 317170.0, 310130.0, 311410.0, 312050.0, 313590.0, 315260.0, 311550.0]</t>
-  </si>
-  <si>
-    <t>[210945.0, 210020.0, 211120.0, 211130.0, 210750.0]</t>
-  </si>
-  <si>
-    <t>[521090.0, 521860.0, 521870.0, 521486.0, 522015.0, 521890.0, 521385.0, 522028.0, 522157.0, 520495.0, 520500.0, 521015.0, 522170.0, 520640.0, 521935.0, 521690.0, 520540.0, 520945.0, 521970.0, 521470.0]</t>
-  </si>
-  <si>
-    <t>[520320.0, 521060.0, 521180.0, 521945.0, 522230.0, 521560.0, 521305.0, 520860.0]</t>
-  </si>
-  <si>
-    <t>[355030.0]</t>
-  </si>
-  <si>
-    <t>[313480.0, 313290.0, 314320.0, 316470.0, 315290.0, 316510.0]</t>
-  </si>
-  <si>
-    <t>[221120.0, 221063.0, 220080.0, 220115.0, 220890.0]</t>
-  </si>
-  <si>
-    <t>[316800.0, 314465.0, 315560.0, 313065.0, 310665.0, 317065.0, 314345.0, 316045.0, 316270.0, 312087.0]</t>
-  </si>
-  <si>
-    <t>[150375.0, 150503.0, 150100.0, 150805.0, 150360.0, 150619.0]</t>
-  </si>
-  <si>
-    <t>[290080.0, 290690.0, 291845.0, 292550.0, 291560.0, 292200.0, 292300.0, 293325.0, 292110.0, 293135.0, 291280.0, 291600.0, 291890.0]</t>
-  </si>
-  <si>
-    <t>[510624.0, 510305.0, 510370.0, 510850.0, 510724.0, 510790.0, 510792.0, 510830.0, 510800.0, 510452.0, 510454.0, 510776.0, 510525.0, 510622.0]</t>
-  </si>
-  <si>
-    <t>[313920.0, 314530.0, 312675.0, 313700.0, 310470.0, 314535.0, 315240.0, 316555.0, 310285.0, 316860.0, 314620.0]</t>
-  </si>
-  <si>
-    <t>[211090.0, 210660.0, 211220.0, 210780.0]</t>
-  </si>
-  <si>
-    <t>[150400.0, 150210.0, 150470.0, 150120.0, 150130.0, 150010.0, 150520.0, 150330.0, 150460.0]</t>
-  </si>
-  <si>
-    <t>[130210.0, 130280.0, 130220.0, 130002.0, 130420.0, 130426.0]</t>
-  </si>
-  <si>
-    <t>[353630.0, 353700.0, 351620.0, 354310.0, 354950.0, 352370.0, 354360.0, 351320.0, 352540.0, 354270.0]</t>
-  </si>
-  <si>
-    <t>[316930.0, 316520.0, 311070.0, 316080.0, 311090.0, 311390.0]</t>
-  </si>
-  <si>
-    <t>[500290.0, 500100.0, 500230.0, 500780.0, 500755.0, 500020.0, 500630.0, 500440.0, 500830.0, 500190.0]</t>
-  </si>
-  <si>
-    <t>[316940.0, 310710.0, 315830.0, 313050.0, 311870.0]</t>
-  </si>
-  <si>
-    <t>[353600.0, 354180.0, 354380.0, 355500.0, 351920.0, 350580.0, 351900.0, 350335.0]</t>
-  </si>
-  <si>
-    <t>[314180.0, 316970.0, 313835.0, 310445.0, 317107.0, 313652.0, 311610.0, 311230.0]</t>
-  </si>
-  <si>
-    <t>[311140.0, 315690.0, 311820.0, 317010.0, 311730.0, 310070.0, 317110.0, 312125.0]</t>
-  </si>
-  <si>
-    <t>[316960.0, 314500.0, 310375.0, 314280.0, 311500.0, 310350.0, 313070.0, 315280.0, 317020.0]</t>
-  </si>
-  <si>
-    <t>[312840.0, 312330.0, 317200.0, 316570.0, 315310.0, 312880.0, 314160.0, 316730.0, 315580.0, 316990.0, 312900.0, 312400.0, 310870.0, 316900.0, 315630.0, 311670.0, 316790.0, 316150.0, 315130.0, 312190.0]</t>
-  </si>
-  <si>
-    <t>[310945.0, 310820.0, 314437.0, 317047.0, 314700.0, 312620.0, 317040.0, 310930.0, 310450.0, 315445.0, 312247.0, 311615.0]</t>
-  </si>
-  <si>
-    <t>[354625.0, 350590.0, 354790.0, 351090.0, 350100.0, 350940.0, 350780.0]</t>
-  </si>
-  <si>
-    <t>[220385.0, 220995.0, 220280.0, 220965.0, 220937.0, 220490.0, 221097.0, 220207.0, 220210.0, 220277.0, 220950.0, 221080.0, 220155.0, 220700.0]</t>
-  </si>
-  <si>
-    <t>[110008.0, 110149.0, 110150.0]</t>
-  </si>
-  <si>
-    <t>[110026.0, 110060.0, 110094.0, 110002.0, 110070.0, 110040.0, 110140.0, 110045.0, 110013.0]</t>
-  </si>
-  <si>
-    <t>[351140.0, 355300.0, 350310.0, 350055.0, 350500.0, 353880.0, 353580.0, 351260.0, 355120.0, 350450.0, 351540.0, 351925.0, 355380.0, 352180.0, 352280.0, 355420.0, 352860.0]</t>
-  </si>
-  <si>
-    <t>[354820.0, 353800.0, 354860.0, 353230.0, 355410.0, 354230.0, 352630.0, 355000.0, 350970.0, 355480.0]</t>
-  </si>
-  <si>
-    <t>[510560.0, 510626.0, 510410.0, 510642.0, 510805.0]</t>
-  </si>
-  <si>
-    <t>[352610.0, 353720.0, 352042.0, 352330.0, 352460.0, 355180.0, 352990.0, 350540.0, 350925.0, 350990.0, 352120.0, 353620.0, 354260.0, 351480.0, 352030.0]</t>
-  </si>
-  <si>
-    <t>[220800.0, 220420.0, 220935.0, 220940.0, 220173.0, 221070.0, 220430.0, 220435.0, 220180.0, 220820.0, 221093.0, 220327.0, 220720.0, 220209.0, 220595.0, 220340.0, 220213.0, 220985.0, 220605.0, 220095.0, 220480.0, 220865.0, 220755.0, 220500.0, 221020.0, 221150.0, 220255.0, 220515.0, 220005.0, 221030.0, 221160.0, 220777.0, 220650.0, 220520.0, 220780.0, 221037.0, 220910.0, 221170.0, 220025.0, 220027.0, 220157.0, 220415.0]</t>
-  </si>
-  <si>
-    <t>[220960.0, 221130.0, 220810.0, 221038.0, 220559.0, 220400.0, 220690.0, 220915.0, 221140.0, 220117.0, 220470.0, 220090.0, 220860.0, 220350.0]</t>
-  </si>
-  <si>
-    <t>[510680.0, 510794.0, 510627.0, 510510.0]</t>
-  </si>
-  <si>
-    <t>[220170.0, 220560.0, 220450.0, 221090.0, 220198.0, 221095.0, 220970.0, 220590.0, 220855.0, 220600.0, 220730.0, 220735.0, 220225.0, 220100.0, 220230.0, 221010.0, 220887.0, 220380.0, 220510.0, 220900.0, 220390.0, 221039.0, 220785.0, 220530.0, 220793.0, 220410.0, 220795.0, 220670.0]</t>
-  </si>
-  <si>
-    <t>[293120.0, 292260.0, 293350.0, 293160.0, 293290.0, 290540.0, 291120.0, 291345.0, 291730.0, 292275.0, 290580.0, 292467.0]</t>
-  </si>
-  <si>
-    <t>[316200.0, 312360.0, 317070.0, 314260.0, 311900.0]</t>
-  </si>
-  <si>
-    <t>[317120.0, 313760.0, 316295.0, 311787.0, 314930.0, 315900.0, 314110.0]</t>
-  </si>
-  <si>
-    <t>[210240.0, 211170.0, 210760.0, 211050.0, 210250.0, 210830.0, 211280.0, 210135.0, 210745.0, 210650.0, 211100.0]</t>
-  </si>
-  <si>
-    <t>[290689.0, 292500.0, 291995.0, 292510.0, 290350.0, 292145.0, 290870.0, 292665.0, 293180.0, 290120.0, 293330.0, 290515.0, 290900.0, 292570.0, 290395.0, 291040.0, 290670.0, 290290.0, 292470.0]</t>
-  </si>
-  <si>
-    <t>[314880.0, 311170.0, 310370.0, 317130.0, 311020.0, 314830.0, 316850.0, 316380.0, 315230.0]</t>
-  </si>
-  <si>
-    <t>[351680.0, 355710.0, 350180.0, 351290.0, 351590.0, 350120.0, 352810.0, 351690.0, 353100.0, 353260.0, 354030.0, 351070.0, 354420.0, 353625.0, 355610.0, 355130.0, 352830.0]</t>
-  </si>
-  <si>
-    <t>[421910.0, 420253.0, 420768.0, 420517.0, 420010.0, 421165.0, 420530.0, 420917.0, 421690.0, 421950.0, 421055.0, 421185.0, 421575.0, 420560.0, 420945.0, 421970.0, 421340.0, 420445.0, 421610.0, 421227.0, 420350.0]</t>
-  </si>
-  <si>
-    <t>[150172.0, 150085.0, 150060.0, 150445.0, 150835.0, 150548.0, 150780.0, 150590.0, 150815.0]</t>
-  </si>
-  <si>
-    <t>[110145.0, 110050.0, 110090.0, 110028.0, 110029.0, 110001.0, 110037.0, 110014.0]</t>
-  </si>
-  <si>
-    <t>[210467.0, 210565.0, 210087.0, 211400.0, 210632.0, 210055.0, 210923.0, 210315.0, 210317.0, 210637.0, 210735.0, 210290.0, 210260.0, 210197.0, 211003.0, 210620.0, 210430.0]</t>
-  </si>
-  <si>
-    <t>[314625.0, 315650.0, 312707.0, 314537.0, 315700.0, 315737.0]</t>
-  </si>
-  <si>
-    <t>[420450.0, 421635.0, 421060.0, 420650.0, 421740.0, 420210.0, 420890.0]</t>
-  </si>
-  <si>
-    <t>[312705.0, 314850.0, 313890.0, 310660.0, 317030.0, 310090.0, 312015.0, 315765.0]</t>
-  </si>
-  <si>
-    <t>[160005.0, 160015.0, 160021.0, 160053.0, 160023.0, 160025.0, 160030.0]</t>
-  </si>
-  <si>
-    <t>[160070.0, 160010.0, 160050.0, 160020.0, 160055.0]</t>
-  </si>
-  <si>
-    <t>[160080.0, 160040.0, 160027.0, 160060.0]</t>
+    <t>[410754, 410500, 410630, 411275, 411670, 410530, 410405, 410930, 412855, 411065, 412090, 410305, 410820, 411345, 410712, 410460, 412382, 410975, 410335, 410345, 410480, 412785, 412402, 410105, 411005]</t>
+  </si>
+  <si>
+    <t>[250915, 251620, 251398, 251420, 251720, 250840, 251320, 251000, 250077]</t>
+  </si>
+  <si>
+    <t>[230690, 230600, 230760, 231080, 231310, 231150, 231250, 231123, 230070, 230680, 230427]</t>
+  </si>
+  <si>
+    <t>[270240, 270330, 270500, 270642, 270580, 270710, 270010]</t>
+  </si>
+  <si>
+    <t>[412800, 410755, 411400, 410250, 410770, 410390, 411295, 410655, 412065, 411680, 412720, 410170, 410300, 410045, 410430, 411080, 412110, 411220, 411610, 412250, 412135, 411880, 410860, 411373, 410750]</t>
+  </si>
+  <si>
+    <t>[251660, 250670, 250800, 250900, 250010, 251230, 251455]</t>
+  </si>
+  <si>
+    <t>[230400, 231170, 230800, 231200, 230050, 230435, 230820, 230310, 230450, 231220, 230580, 231095, 230465, 230990, 230610, 230490, 230365, 231390, 230880, 231395, 231280, 230900, 230520, 231290]</t>
+  </si>
+  <si>
+    <t>[410752, 412810, 412690, 411155, 410660, 411060, 412862, 410050, 411720, 411470, 412880, 410832, 410070, 410337, 410725, 410347, 411885, 410990, 411890, 411510, 412535]</t>
+  </si>
+  <si>
+    <t>[250720, 250690, 250790, 250760, 251275, 250380, 251500, 251310, 251150, 251120, 250640, 251445, 250680, 250940]</t>
+  </si>
+  <si>
+    <t>[230020, 230725, 230890, 230230, 230425, 230780, 230655]</t>
+  </si>
+  <si>
+    <t>[411040, 410560, 412610, 412260, 411300, 412680, 411240, 412555, 410550, 412790, 410910]</t>
+  </si>
+  <si>
+    <t>[251392, 251396, 250375, 251210, 251090, 250810]</t>
+  </si>
+  <si>
+    <t>[231360, 230530, 230500, 230340, 231340, 231410, 230423, 231230]</t>
+  </si>
+  <si>
+    <t>[411650, 412420, 410890, 411030, 411800, 412330, 412460, 412590, 410670, 411830, 412730, 411710, 411840, 411970, 412100, 411590, 412490, 410060, 412370, 410710, 411350, 410090, 412395, 411500, 412020, 411130, 411260, 412670]</t>
+  </si>
+  <si>
+    <t>[250403, 251272, 250890, 250730, 250930, 250710, 250905, 251290, 250523, 250140, 250527]</t>
+  </si>
+  <si>
+    <t>[230040, 231330, 231030, 230150]</t>
+  </si>
+  <si>
+    <t>[411520, 410115, 412040, 411410, 411160, 411640, 410780, 411420, 412830, 412450, 411810, 410790, 411690, 412340, 410810, 412360, 412625, 411090, 411480, 411740, 410590, 411360, 410210, 411750, 411110, 410730, 410220, 411630, 412530, 411000]</t>
+  </si>
+  <si>
+    <t>[250625, 251394, 250435, 250053, 250310, 250250, 250157, 251278, 250990, 251250, 250130, 251700, 251315, 250170]</t>
+  </si>
+  <si>
+    <t>[230560, 230565, 230410, 230860, 230125, 230930, 231126, 231320, 231100, 230940, 230590]</t>
+  </si>
+  <si>
+    <t>[411490, 412580, 410150, 410760, 411210, 410380, 411310, 410350, 410320, 411729, 412210, 412270, 410870, 411575, 410330, 410140, 411550]</t>
+  </si>
+  <si>
+    <t>[251200, 250400, 251650, 250850, 250215, 251240, 250920, 251050, 250610, 250770, 250135, 251385, 251610, 251675, 251580]</t>
+  </si>
+  <si>
+    <t>[230470, 230790, 230260, 230390, 230205]</t>
+  </si>
+  <si>
+    <t>[412033, 410370, 411270, 410510, 412050, 410920, 410280, 410800, 411190, 411965, 410190, 411600, 412240, 410080, 412000, 410980, 410340, 412650, 411370, 411380, 412667]</t>
+  </si>
+  <si>
+    <t>[230180, 230950, 230570, 231370, 230540, 230380, 230750]</t>
+  </si>
+  <si>
+    <t>[410240, 411660, 412430, 410640, 412310, 410010, 412190, 412320, 412840, 411700, 412470, 412600, 411721, 412620, 411340, 411100, 412640, 412130, 412390, 410600, 410110]</t>
+  </si>
+  <si>
+    <t>[230330, 230850, 230030, 231090, 230740, 230550, 231190, 230360, 230426, 231135]</t>
+  </si>
+  <si>
+    <t>[412290, 411920, 411280, 412180, 410900, 410775, 411290, 410270, 411170, 412070, 411180, 412850, 410970, 411230, 410470, 412780, 412400, 410610, 412660, 410360, 412410, 412540]</t>
+  </si>
+  <si>
+    <t>[230720, 231110, 230250, 230830, 230810, 231060, 230200, 230010, 230170]</t>
+  </si>
+  <si>
+    <t>[411620, 410950, 410120, 411820, 410960, 411570, 411995]</t>
+  </si>
+  <si>
+    <t>[230440, 230625, 230100, 230428]</t>
+  </si>
+  <si>
+    <t>[250180, 251370, 251530, 251276, 250860, 250060, 251597, 250320, 251190, 250910, 250490, 250300, 250750, 250460]</t>
+  </si>
+  <si>
+    <t>[270690, 270050, 270470, 270790, 270280, 270890, 270220, 270060, 270770, 270644, 270520, 270430]</t>
+  </si>
+  <si>
+    <t>[240770, 241420, 240140, 240910, 240780, 240660, 240790, 240920, 240420, 241320, 241330, 240180, 240820, 241470, 240830, 241220, 241350, 241480, 240980, 241500, 240220, 240350, 240615, 240620, 240630, 240120, 241150]</t>
+  </si>
+  <si>
+    <t>[410880, 410753, 411585, 412545, 411460, 411845, 411745, 412740, 412770, 411722, 412795, 411790, 411535, 412085, 410200, 410715, 412350, 412575]</t>
+  </si>
+  <si>
+    <t>[230080, 231400, 230920, 231210, 230060, 230160, 231120, 230130, 230420, 230430, 231195, 231325, 230270]</t>
+  </si>
+  <si>
+    <t>[412710, 412170, 410700, 412750, 411730, 412853, 411007]</t>
+  </si>
+  <si>
+    <t>[230730, 230190, 230480, 230320, 230710, 230840]</t>
+  </si>
+  <si>
+    <t>[412385, 410855, 410440, 410185, 412265, 411150, 411375, 411727, 411342, 411250, 412500, 410165, 411573, 412217, 411450, 410685]</t>
+  </si>
+  <si>
+    <t>[230945, 230523, 230220, 231085, 230350, 230960, 230395]</t>
+  </si>
+  <si>
+    <t>[411910, 412550, 411915, 410765, 410520, 410400, 410020, 411430, 410410, 410030, 411950, 412080, 410420, 410040, 410425, 411320, 412220, 412863, 410690, 410180, 412230, 410310, 410580, 412760, 412120, 412788, 411125, 410230, 410620]</t>
+  </si>
+  <si>
+    <t>[250630, 251274, 251640, 250520, 251160, 250270, 251170, 250150, 251560, 251180, 250415, 250050, 250820, 251590, 251593, 250570, 250190, 251600, 250580, 250080, 250980, 250855, 250350, 250100, 250360]</t>
+  </si>
+  <si>
+    <t>[230370, 230630, 231335, 231240, 230090, 231020, 230460, 231025, 231260, 231070]</t>
+  </si>
+  <si>
+    <t>[270850, 270730, 270510, 270350, 270450, 270740, 270870, 270360, 270650]</t>
+  </si>
+  <si>
+    <t>[240800, 240130, 240100, 240230, 240520, 240430, 240110, 241105, 240370, 240440, 241460, 240145, 241335, 240760]</t>
+  </si>
+  <si>
+    <t>[411200, 410465, 411140, 411940, 411770, 411050, 412010, 410160, 412630, 411990, 410490, 412510]</t>
+  </si>
+  <si>
+    <t>[251270, 250950, 250120, 250057, 250090, 250600, 250830, 250030, 250933, 251510, 250040, 250110]</t>
+  </si>
+  <si>
+    <t>[231010, 230765, 230015, 230770, 230195, 231160, 230970, 230495]</t>
+  </si>
+  <si>
+    <t>[270560, 270210, 270380, 270830, 270930, 270390, 270135, 270550, 270810, 270300, 270110]</t>
+  </si>
+  <si>
+    <t>[240260, 241160, 241040, 240410, 240670, 240030, 241440, 240160, 240550, 240950, 240185, 240190, 240960, 241090, 240450, 240580, 240970, 240460, 240720, 241255, 241390, 240750, 240880, 241010, 240510, 240895]</t>
+  </si>
+  <si>
+    <t>[411010, 412200, 411020, 411390, 410895, 410773, 412150, 412700, 411070]</t>
+  </si>
+  <si>
+    <t>[251010, 250500, 251140, 251110, 250535, 250153, 250510, 250160, 251540, 251030, 250620, 251615]</t>
+  </si>
+  <si>
+    <t>[230210, 230980, 230120, 230510, 230290, 230650, 230140, 230910]</t>
+  </si>
+  <si>
+    <t>[270660, 270490, 270760, 270700, 270190, 270130, 270040, 270170, 270940]</t>
+  </si>
+  <si>
+    <t>[241415, 240650, 240010, 240270, 241300, 241430, 241180, 240165, 240300, 240560, 240310, 241210, 240570, 241340, 240200, 240850, 240340, 241240, 240480, 240610, 240240, 241140, 241142, 240890, 240380]</t>
+  </si>
+  <si>
+    <t>[411780, 412175, 411545, 411930, 410395, 412060, 412215, 411960, 411705, 410940, 411325, 410304, 412865, 411330, 410442, 410445, 410845, 412015, 410865, 412796]</t>
+  </si>
+  <si>
+    <t>[251520, 251065, 250970, 250470, 250407, 251400, 251630, 251410, 251220, 250485, 250390, 251060, 251480, 250073, 250650, 251740, 251550]</t>
+  </si>
+  <si>
+    <t>[230240, 231040, 230660, 230280, 230763, 230300]</t>
+  </si>
+  <si>
+    <t>[270400, 270915, 270020, 270140, 270860, 270100, 270780]</t>
+  </si>
+  <si>
+    <t>[240640, 241030, 241290, 241170, 240530, 240150, 240280, 240540, 241310, 240933, 240680, 240170, 241230, 240210, 241110, 241370, 241120, 241260, 240500, 241270, 241400]</t>
+  </si>
+  <si>
+    <t>[412030, 410850, 412560, 410290, 410130, 412820, 411860, 410680, 411870]</t>
+  </si>
+  <si>
+    <t>[250880, 250115, 251670, 250780, 251300, 250540, 251440, 250420, 250550, 250939, 251070, 251710, 251460, 251080, 251340, 251470, 250450, 250590, 251490, 250340, 250355, 251380, 250870, 251260]</t>
+  </si>
+  <si>
+    <t>[231355, 231375, 230640, 231380, 230837, 231350, 230075]</t>
+  </si>
+  <si>
+    <t>[270820, 270375, 270670, 270320, 270270, 270230, 270680, 270750]</t>
+  </si>
+  <si>
+    <t>[241410, 240390, 240400, 241050, 240930, 240290, 241060, 241190, 240040, 241450, 240940, 241070, 240690, 240050, 241080, 240700, 240060, 240320, 241475, 240840, 240330, 241355, 241100, 240590, 241360, 241490, 240725, 240600, 240090, 240730, 240860, 241250, 241380, 240740, 241000, 240490, 241020]</t>
+  </si>
+  <si>
+    <t>[412480, 412870, 410570, 411530, 410540, 411850, 411120, 411760, 410322, 412627, 411440, 410965, 410645, 412665, 410650]</t>
+  </si>
+  <si>
+    <t>[250560, 251360, 250210, 250530, 250020, 251040, 250660, 251335, 250440, 251430, 251020, 250700, 250480, 251570, 250260, 251350, 251130, 251100]</t>
+  </si>
+  <si>
+    <t>[230620, 230445, 230110, 230535]</t>
+  </si>
+  <si>
+    <t>[270880, 270370, 270340, 270150, 270920, 270440, 270090, 270410, 270030, 270290, 270420, 270260, 270070, 270200, 270235, 270910, 270590]</t>
+  </si>
+  <si>
+    <t>[240325, 240710, 240360, 240810, 241200]</t>
+  </si>
+  <si>
+    <t>[412160, 412035, 412300, 411540, 410260, 411925, 412440, 410657, 410785, 410275, 411435, 411695, 412860, 410302, 410315, 411980, 411725, 410450, 410840, 412380, 410720, 412520, 412140, 410100, 410740, 412280, 411900]</t>
+  </si>
+  <si>
+    <t>[250280, 251465, 250430, 251280, 250290, 250740, 250230, 250200, 250937, 251390]</t>
+  </si>
+  <si>
+    <t>[231300, 231140, 231270, 230533, 230185, 231050, 230835, 230393, 231130, 230526]</t>
+  </si>
+  <si>
+    <t>[270080, 270530, 270630, 270310, 270120, 270255, 270480, 270900]</t>
+  </si>
+  <si>
+    <t>[241280, 241025, 240485, 240870, 240070, 241445, 240080, 240020, 240470, 240375, 240250, 240990]</t>
+  </si>
+  <si>
+    <t>[411560, 410830, 412405, 411605, 411095, 412570, 412635, 411580, 412125]</t>
+  </si>
+  <si>
+    <t>[250240, 251680, 250370, 251330, 251203, 251365, 251207, 250410, 251690, 250220, 250960, 251450, 250070, 250330, 250205]</t>
+  </si>
+  <si>
+    <t>[230700, 231180, 230670, 230870, 231000]</t>
+  </si>
+  <si>
+    <t>[270720, 270180, 270600, 270570, 270250, 270540, 270895, 270800, 270160, 270610, 270640, 270620, 270840, 270460]</t>
+  </si>
+  <si>
+    <t>[352740, 354085, 354470, 354510, 351600, 352080, 353490, 353460, 352890, 350010]</t>
+  </si>
+  <si>
+    <t>[261440, 261153, 260770, 261280, 260390, 260710, 260010, 261360, 260690, 261460, 261590, 260250]</t>
+  </si>
+  <si>
+    <t>[291650, 291590, 292970, 291370, 291050, 290220, 291790, 290700, 290960, 292330, 290030, 290190, 291060, 290070, 292410, 292700, 290205, 290750]</t>
+  </si>
+  <si>
+    <t>[314720, 315170, 310530, 312520, 313900, 311470, 312240, 310160, 316690, 311160, 310200, 310840, 311130, 310430, 311100, 311710]</t>
+  </si>
+  <si>
+    <t>[313600, 315710, 315810, 314055, 315660, 313580, 312560, 313650, 314675, 315510, 310520, 313470, 316030, 310170]</t>
+  </si>
+  <si>
+    <t>[352130, 353190, 353360, 353430, 354490, 354940]</t>
+  </si>
+  <si>
+    <t>[350820, 352410, 352010, 352970, 351770, 350300]</t>
+  </si>
+  <si>
+    <t>[352160, 353540, 353160, 353640, 353480, 351440, 354930, 355510, 354710, 352600, 351580, 353310]</t>
+  </si>
+  <si>
+    <t>[353920, 350080, 354830, 354323, 351512, 352920, 350240, 351530, 350890, 350130, 352060, 355390, 354240, 353220, 354120, 354770, 355290, 354140, 354550]</t>
+  </si>
+  <si>
+    <t>[120025, 120010, 120005, 120070]</t>
+  </si>
+  <si>
+    <t>[354220, 352560, 351990, 354170, 353215]</t>
+  </si>
+  <si>
+    <t>[130370, 130020, 130406, 130060, 130160, 130390, 130423, 130006, 130230]</t>
+  </si>
+  <si>
+    <t>[510080, 510629, 510279, 510025, 510895, 510615]</t>
+  </si>
+  <si>
+    <t>[420800, 420770, 421960, 420075, 420780, 421260, 420430, 421390, 421750, 420760, 420985, 421310, 420127]</t>
+  </si>
+  <si>
+    <t>[420740, 421780, 421270, 421400, 421530, 420510, 421920, 421410, 421935, 420915, 420020, 421940, 420285, 420030, 421567, 420419, 421450, 420690, 420180, 421460, 420950, 421085, 420190, 421860, 421480, 420850, 421370, 420990]</t>
+  </si>
+  <si>
+    <t>[353560, 350850, 354600, 352490, 354990, 353170, 352020, 352440]</t>
+  </si>
+  <si>
+    <t>[420480, 421005, 420757, 421790, 421540, 421930, 421550, 421300, 421440, 420160, 421825, 420675, 420550, 420555, 420300, 421070, 421335, 420315, 421605, 420970]</t>
+  </si>
+  <si>
+    <t>[354500, 353060, 354680, 350660, 351880, 355250, 351570, 351830, 352310, 350390, 353980]</t>
+  </si>
+  <si>
+    <t>[316000, 310150, 315110, 312460, 317210]</t>
+  </si>
+  <si>
+    <t>[171360, 172065, 170370, 170755, 170980, 171270, 171820, 170510, 171790, 171890, 171700, 171420, 171550]</t>
+  </si>
+  <si>
+    <t>[354340, 354750, 355140, 354760, 351885, 351310, 355150, 355090, 352760, 352510]</t>
+  </si>
+  <si>
+    <t>[280320, 280030, 280200, 280360, 280650, 280590, 280060, 280670]</t>
+  </si>
+  <si>
+    <t>[150304, 150658, 150840, 150276, 150555, 150730, 150125, 150670, 150543, 150034, 150613, 150775, 150808, 150616, 150270]</t>
+  </si>
+  <si>
+    <t>[510860, 510735, 510677, 510774, 510777, 510269, 510335]</t>
+  </si>
+  <si>
+    <t>[353930, 351220, 350330, 354620, 352670]</t>
+  </si>
+  <si>
+    <t>[310400, 314980, 315300, 314920, 316810, 311150, 312950, 315770]</t>
+  </si>
+  <si>
+    <t>[310340, 317160, 313545, 312650, 311950, 310650]</t>
+  </si>
+  <si>
+    <t>[261600, 261410, 260805, 261480, 261580, 261100, 260915, 260660, 260280, 261080, 260120, 260700, 260510]</t>
+  </si>
+  <si>
+    <t>[350720, 350400, 351330, 355395, 353530, 353550, 352880, 353970, 353715, 352790, 351000, 351610]</t>
+  </si>
+  <si>
+    <t>[211085, 210542, 211153, 210005, 211285, 210325, 210232, 210203]</t>
+  </si>
+  <si>
+    <t>[211300, 211140, 210215, 210120, 210635, 210355, 210740, 210040, 210810, 210590, 210207]</t>
+  </si>
+  <si>
+    <t>[330380, 330010, 330260]</t>
+  </si>
+  <si>
+    <t>[353080, 355730, 352260, 353070]</t>
+  </si>
+  <si>
+    <t>[510620, 510340, 510010, 510650, 510160, 510610, 510645, 510300, 510840, 510490, 510780]</t>
+  </si>
+  <si>
+    <t>[330020, 330023, 330025, 330187, 330130, 330452, 330070, 330550, 330520]</t>
+  </si>
+  <si>
+    <t>[353760, 354850, 350635, 352210, 354100, 351350, 353110, 355100, 351870]</t>
+  </si>
+  <si>
+    <t>[120032, 120001, 120034, 120038, 120040, 120043, 120045, 120013, 120080, 120017, 120050]</t>
+  </si>
+  <si>
+    <t>[130050, 130340, 130290, 130068, 130300]</t>
+  </si>
+  <si>
+    <t>[150145, 150050, 150530, 150565, 150600, 150475, 150285, 150510, 150797, 150480, 150390, 150040, 150300, 150680]</t>
+  </si>
+  <si>
+    <t>[211200, 210050, 210725, 210950, 210407, 211080, 210409, 210410, 210610, 211157, 211160, 210970, 210140]</t>
+  </si>
+  <si>
+    <t>[310560, 310210, 315940, 314660, 316620, 312940, 311630, 315440, 315730, 310163, 311220, 310290, 312150, 311320, 315870]</t>
+  </si>
+  <si>
+    <t>[210535, 210408, 210095, 210160, 210480, 210547]</t>
+  </si>
+  <si>
+    <t>[293345, 293090, 291110, 290970, 292840, 290440, 290250, 292620, 292045, 290940, 290320, 291955, 290740, 292890, 290140]</t>
+  </si>
+  <si>
+    <t>[352800, 353890, 350340, 351910, 353670, 352680, 353657, 354250, 350470, 350600, 352750, 350830, 353940, 350070, 350745, 351450, 350430, 354110]</t>
+  </si>
+  <si>
+    <t>[316830, 315780, 315460, 310620, 310640, 314480, 313460, 315670, 314230, 311000, 315480, 313660, 315390]</t>
+  </si>
+  <si>
+    <t>[315040, 313665, 316292, 312410, 315530, 310670, 313010, 310900, 314070, 312600, 310810, 312060, 314015]</t>
+  </si>
+  <si>
+    <t>[170380, 170382, 170255, 171280, 170389, 171430, 170030, 172080, 170290, 171830, 171070, 171855, 172120, 172000, 171880, 172010, 170220, 171245, 170740, 172020, 170100, 171380, 170105, 172030]</t>
+  </si>
+  <si>
+    <t>[313640, 310730, 314545, 312660, 312825, 312380]</t>
+  </si>
+  <si>
+    <t>[314240, 312320, 314050, 310740, 316660, 312470, 313880]</t>
+  </si>
+  <si>
+    <t>[353860, 352550, 355495, 350760, 355210, 350410, 353680, 355635, 350710, 353240, 353820]</t>
+  </si>
+  <si>
+    <t>[317090, 316420, 312965, 317000, 313865, 311115, 313868, 310860, 316110, 313005, 316240, 315057, 314795, 317052, 313535]</t>
+  </si>
+  <si>
+    <t>[290050, 292360, 291720, 291980, 291860, 291220, 290200, 290460, 291250, 292670, 292030, 290880, 291010, 290755, 292690, 291165, 290280, 290410, 293100, 291950]</t>
+  </si>
+  <si>
+    <t>[110018, 110147, 110148, 110120, 110004, 110009]</t>
+  </si>
+  <si>
+    <t>[292100, 292520, 290570, 290860, 293070, 291005]</t>
+  </si>
+  <si>
+    <t>[310080, 311200, 311040, 315880, 311120, 312020, 311190]</t>
+  </si>
+  <si>
+    <t>[500740, 500490, 500110, 500750, 500627, 500500, 500640, 500769, 500260, 500390, 500270, 500790, 500150, 500280, 500025, 500793, 500410, 500540, 500800, 500295, 500560, 500690, 500220, 500310, 500580, 500325, 500070, 500710, 500330, 500210, 500215, 500600, 500730, 500348]</t>
+  </si>
+  <si>
+    <t>[170720, 171845, 170310, 171750, 170025, 171370, 171500, 170190, 171250, 170610, 170390, 171190, 170710, 171610, 170460]</t>
+  </si>
+  <si>
+    <t>[171200, 171330, 171875, 172100, 171240, 170825, 172110, 172015, 171510, 171320, 170110, 171195, 171900, 171870]</t>
+  </si>
+  <si>
+    <t>[150497, 150370, 150563, 150277, 150215, 150553, 150157, 150420, 150293, 150549, 150295, 150745, 150618, 150715, 150013, 150750, 150175]</t>
+  </si>
+  <si>
+    <t>[311330, 311010, 312420, 312200, 311210, 314587, 312530, 312595, 314900, 316920, 314875]</t>
+  </si>
+  <si>
+    <t>[312385, 313090, 316447, 317057, 315015, 311340, 315725, 315935, 317005, 316095, 317115, 310780, 313055]</t>
+  </si>
+  <si>
+    <t>[421760, 420545, 420960, 421120, 421160, 420425, 421835, 421900, 420460, 422000, 421170, 420700]</t>
+  </si>
+  <si>
+    <t>[220194, 220675, 220260, 220551, 220105, 220202, 221065, 220205, 220527, 221040, 220271, 220177, 220695, 220220, 220990]</t>
+  </si>
+  <si>
+    <t>[261120, 261250, 260230, 260500, 261270, 261020, 260640, 260130, 260260, 261540, 261170, 261300, 260410, 260030, 261310, 260800, 260670, 260170, 261200, 261330, 260310, 260060, 260190, 261470, 261090, 260580, 260840, 260080, 261620, 261240, 261500, 260350]</t>
+  </si>
+  <si>
+    <t>[311240, 312970, 312120, 311510, 311640]</t>
+  </si>
+  <si>
+    <t>[354560, 351492, 351110, 351495, 351120, 355600, 353810, 352150, 353570, 350370, 353325, 354480, 355260, 352190, 353350, 351560, 353510, 353900, 352885]</t>
+  </si>
+  <si>
+    <t>[211107, 210340, 210220, 210030, 210390, 210010, 210300]</t>
+  </si>
+  <si>
+    <t>[521990, 520460, 521500, 522140, 520870, 520360, 521000, 520880, 521140, 521910, 520130, 521540, 520005, 520520, 521680, 520920, 520280, 521950, 520160, 521440, 521056, 520680, 521450, 522100, 521205, 521973]</t>
+  </si>
+  <si>
+    <t>[110180, 110025, 110155, 110143, 110175, 110032, 110160, 110034, 110130, 110100, 110170, 110011, 110012, 110015]</t>
+  </si>
+  <si>
+    <t>[320515, 320517, 320390, 320013, 320400, 320016, 320405, 320150, 320410, 320160, 320035, 320425, 320305, 320435, 320320, 320330, 320335, 320080, 320465, 320210, 320470, 320090, 320350, 320225, 320100, 320360, 320490, 320495, 320501]</t>
+  </si>
+  <si>
+    <t>[353286, 350280, 354440, 351820, 355630, 350640, 353330, 351890, 350420, 354805, 350620]</t>
+  </si>
+  <si>
+    <t>[354690, 354370, 351685, 350670, 350320, 355475, 353205, 350170]</t>
+  </si>
+  <si>
+    <t>[510050, 510600, 510890, 510730, 510350, 510770, 510590]</t>
+  </si>
+  <si>
+    <t>[140002, 140005, 140070, 140040, 140010, 140045, 140015, 140017, 140030]</t>
+  </si>
+  <si>
+    <t>[355270, 353290, 352270, 350740, 351960]</t>
+  </si>
+  <si>
+    <t>[520455, 520970, 520330, 521230, 520735, 520355, 520995, 520740, 522026, 521770, 521260, 520630, 521530, 522045, 520650, 520140, 522060, 522190, 521170, 522200, 522205, 520545, 521710, 521839, 520180]</t>
+  </si>
+  <si>
+    <t>[330370, 330180, 330022, 330600, 330280, 330540, 330095, 330385, 330290, 330360, 330620]</t>
+  </si>
+  <si>
+    <t>[171650, 171665, 171670, 170410, 171050, 171180, 171570, 170930, 170550, 171840, 170305, 171850, 170830, 170320, 171090, 170330, 172125, 172130, 171110, 170600, 171888, 170230, 170360]</t>
+  </si>
+  <si>
+    <t>[220930, 220290, 221062, 220552, 220300, 220045, 220310, 220440, 220190, 220320, 220323, 220975, 220740, 220870, 220360, 220110, 220885, 220760, 220130, 220275, 220660, 220920, 220665]</t>
+  </si>
+  <si>
+    <t>[210080, 210210, 211010, 210630, 210090, 210667, 211023, 210320, 210640, 211250, 211060, 210805, 210015]</t>
+  </si>
+  <si>
+    <t>[355200, 351840, 351360, 350250, 350315, 351340, 350860, 350350, 354190, 352720, 354960, 350995, 352660, 353850, 350490, 354075, 354430]</t>
+  </si>
+  <si>
+    <t>[353120, 350050, 350190, 355160, 352700]</t>
+  </si>
+  <si>
+    <t>[220545, 220680, 220557, 220830, 220196, 220580, 220840, 220585, 220850, 220342, 220217, 220987, 220610, 220997, 221005, 220240, 220370, 220120, 220635, 220150, 220790, 220667, 220540]</t>
+  </si>
+  <si>
+    <t>[211210, 211150, 210360, 210330, 210043, 210845]</t>
+  </si>
+  <si>
+    <t>[110146, 110092, 110030, 110003, 110005, 110006, 110007]</t>
+  </si>
+  <si>
+    <t>[313540, 312390, 312140, 311800, 316090, 314590]</t>
+  </si>
+  <si>
+    <t>[315520, 311490, 315910, 315080, 312040, 313390, 311310, 315380, 311540, 311830, 316600, 313790]</t>
+  </si>
+  <si>
+    <t>[355520, 352770, 353730, 351650, 351710, 350440, 353770, 350510, 350650, 350770, 351250, 352725, 351190, 350775, 354840, 350810, 350110]</t>
+  </si>
+  <si>
+    <t>[316553, 312980, 311860]</t>
+  </si>
+  <si>
+    <t>[316225, 313730, 311880, 316265, 313560]</t>
+  </si>
+  <si>
+    <t>[351430, 354890, 351370, 354290, 354070, 351930]</t>
+  </si>
+  <si>
+    <t>[312000, 311940, 316870, 315053, 314030, 313500, 312180, 310300]</t>
+  </si>
+  <si>
+    <t>[500520, 500320]</t>
+  </si>
+  <si>
+    <t>[292960, 290980, 290820, 292900, 292230, 290485, 291160, 290490, 292060]</t>
+  </si>
+  <si>
+    <t>[311910, 316935, 310920, 314250, 310480, 315320, 313110, 314360, 312570, 312090, 316060]</t>
+  </si>
+  <si>
+    <t>[312160, 311680, 313250, 311810, 312100, 315330, 312550, 312010, 316590, 311350, 312760, 312540]</t>
+  </si>
+  <si>
+    <t>[530010]</t>
+  </si>
+  <si>
+    <t>[312230, 313350, 311660, 316460, 316180, 310390, 314970, 311420]</t>
+  </si>
+  <si>
+    <t>[500480, 500620, 500240, 500625, 500370, 500375, 500635, 500380, 500124, 500510, 500770, 500515, 500525, 500400, 500660, 500795, 500797, 500430, 500568, 500570, 500315, 500060, 500450, 500840, 500200, 500460, 500720, 500080, 500085, 500470, 500345, 500090, 500350]</t>
+  </si>
+  <si>
+    <t>[521760, 520800, 522220, 522000, 520017, 520400, 520790, 520060]</t>
+  </si>
+  <si>
+    <t>[521250, 520549, 522185, 520620, 521523, 521975, 520025]</t>
+  </si>
+  <si>
+    <t>[220160, 220672, 220550, 220040, 220554, 220555, 220558, 220945, 220050, 220060, 220325, 220710, 220330, 220460, 221100, 220980, 221110, 220620, 220750, 220880, 220630, 220640, 220775, 220010, 220779, 220140, 220525, 220273, 220020, 221050, 220030]</t>
+  </si>
+  <si>
+    <t>[520480, 521920, 520450, 522180, 521480, 521290, 521740, 521580, 520590, 521550, 521010, 520850, 520690, 520660, 522130, 521878, 520120, 520510]</t>
+  </si>
+  <si>
+    <t>[280067, 280040, 280170, 280300, 280750, 280210, 280510, 280630, 280280, 280760]</t>
+  </si>
+  <si>
+    <t>[420490, 421520, 420500, 420765, 421535, 420640, 420257, 421795, 421670, 420775, 421415, 421555, 420660, 420535, 421050, 421568, 421200, 421715, 421720, 421730, 421090, 421223, 420840, 421100, 420080, 420208, 420209, 421875, 420215, 421625]</t>
+  </si>
+  <si>
+    <t>[353830, 354150, 352870, 354130, 350910]</t>
+  </si>
+  <si>
+    <t>[420195, 421380, 421125, 420870, 420519, 421640, 421225, 421770, 420140, 420207, 421040, 421810, 421880, 421080, 421565]</t>
+  </si>
+  <si>
+    <t>[291330, 291080, 292750, 292880, 293140, 292630, 290850, 293040, 292273, 293170, 291380, 291125, 292405, 290110, 292930, 291400, 290890, 290170, 290640, 290260, 292830, 290150, 292465, 292210, 292595, 293110, 291450, 290685]</t>
+  </si>
+  <si>
+    <t>[351520, 352960, 353475, 352070, 353000, 354920, 355530, 354925, 354040, 352820, 351800, 353690, 351550]</t>
+  </si>
+  <si>
+    <t>[312610, 313030, 311980, 310510, 314130, 316820, 314650, 311995]</t>
+  </si>
+  <si>
+    <t>[420320, 421280, 421250, 421350, 420710, 420200, 421000, 421130, 420820, 420245, 420830]</t>
+  </si>
+  <si>
+    <t>[310850, 311270, 312780, 312030, 313657, 312670]</t>
+  </si>
+  <si>
+    <t>[350920, 351630, 352850, 350900, 351640]</t>
+  </si>
+  <si>
+    <t>[313440, 316130, 312710, 313862, 311690, 315160, 317043, 312700, 313340, 315070, 311455]</t>
+  </si>
+  <si>
+    <t>[260100, 261510, 260750, 260880, 260240, 261010, 260370, 260380, 261030, 260650, 261320, 260050, 260825, 260830, 260320, 260330, 261230, 260210, 260470, 260600, 260860]</t>
+  </si>
+  <si>
+    <t>[510625, 510628, 510180, 510820, 510665, 510670, 510100, 510260, 510390, 510719]</t>
+  </si>
+  <si>
+    <t>[260900, 261380, 260070, 260550, 260360, 260780, 260620, 260460, 261530, 260765]</t>
+  </si>
+  <si>
+    <t>[316160, 312580, 316165, 316550, 317190, 316300, 316950, 312730, 314010, 312220, 313507, 310180, 316840, 312750, 312370, 314420, 312770, 317150, 311265, 316770, 315750, 313320, 311920, 312690]</t>
+  </si>
+  <si>
+    <t>[354880, 354410, 352940, 351380, 354870, 354330, 354780]</t>
+  </si>
+  <si>
+    <t>[420230, 420110, 420370, 420120, 421660, 421020, 421150, 421800, 421430, 420540, 421570, 421190, 421590, 420570, 420060, 421725, 420070, 421230, 420980, 420600, 420090, 421630]</t>
+  </si>
+  <si>
+    <t>[291200, 291077, 293000, 292105, 291340, 293260, 291733, 290710, 291740, 292640, 291875, 292020, 290500, 292680, 292180, 290520, 291170, 292450, 291940, 290660, 293105, 290420, 292340]</t>
+  </si>
+  <si>
+    <t>[315680, 312800, 316610, 312260, 314060, 315600, 311380, 312310, 317180]</t>
+  </si>
+  <si>
+    <t>[310950, 312870, 316390, 314410, 310410, 313690, 314300, 312830]</t>
+  </si>
+  <si>
+    <t>[350560, 355170, 354020, 351460, 353130, 354090, 352430, 351860, 353950]</t>
+  </si>
+  <si>
+    <t>[292320, 292225, 292160, 290475, 292370, 290450, 291410, 291320, 290270]</t>
+  </si>
+  <si>
+    <t>[170625, 172097, 170820, 170950, 170730, 171884, 170765, 171150, 171660, 171889, 170386, 170035, 172049, 172085, 170070, 171575, 170200, 172025]</t>
+  </si>
+  <si>
+    <t>[291360, 291490, 293250, 292805, 290630, 290225, 293270, 292090]</t>
+  </si>
+  <si>
+    <t>[211105, 210530, 210405, 210598, 210375, 210280, 211176, 210955, 211180, 210700, 210060, 210255, 210900, 210550, 210455, 210235]</t>
+  </si>
+  <si>
+    <t>[310880, 312250, 312930, 310050, 316260, 314435, 310630, 313610, 313130, 310925, 314995, 315895, 314170, 313115]</t>
+  </si>
+  <si>
+    <t>[291460, 291850, 290323, 291240, 291130, 290620, 292925, 290115, 290760, 291915, 291535, 292560, 290530, 292205, 291310, 293360, 293240, 291835, 290300]</t>
+  </si>
+  <si>
+    <t>[280290, 280100, 280390, 280230, 280680, 280520, 280140, 280370, 280050, 280500, 280600, 280410, 280700, 280445]</t>
+  </si>
+  <si>
+    <t>[293280, 290405, 291500, 290380, 291900, 291470, 292080, 292720, 290130, 291190, 291960, 291260, 293340, 292285]</t>
+  </si>
+  <si>
+    <t>[313280, 316480, 314370, 314750, 315720, 310540, 312590, 311535, 313170, 310770, 316050, 315800, 316190]</t>
+  </si>
+  <si>
+    <t>[290560, 291210, 291855, 291480, 290330, 291100, 291620, 292390, 290470, 290090, 292780, 290240, 291270, 292935, 291660, 291150, 291540, 291550, 293220, 292070, 293230, 290800]</t>
+  </si>
+  <si>
+    <t>[316320, 315100, 312740, 317220, 313990, 311720, 311850, 314730, 310890, 314040, 312110, 315090, 313240, 316540, 314910]</t>
+  </si>
+  <si>
+    <t>[311080, 312680, 316330, 313270, 315000, 314490]</t>
+  </si>
+  <si>
+    <t>[314315, 315217, 313330, 311700, 313400, 314140]</t>
+  </si>
+  <si>
+    <t>[211040, 210720, 210880, 211270, 210663, 210540, 210930, 210675, 210100, 210070, 211290, 211260, 210173, 210270]</t>
+  </si>
+  <si>
+    <t>[291680, 292000, 291970, 291580, 292270, 290480, 291090, 291710, 291350, 291640, 292540, 291230]</t>
+  </si>
+  <si>
+    <t>[350945, 352230, 355110, 355400, 351850, 350220, 351020, 351150, 355020, 354325, 354165, 351160, 350075]</t>
+  </si>
+  <si>
+    <t>[352320, 353282, 350535, 354280, 352265, 352170, 354350, 351760, 352240, 350800, 352215, 355385, 350715, 354300, 350270]</t>
+  </si>
+  <si>
+    <t>[313220, 313370, 315060, 313380]</t>
+  </si>
+  <si>
+    <t>[310980, 311110, 313420, 315980, 312910, 311180, 313140, 311580, 311260]</t>
+  </si>
+  <si>
+    <t>[292480, 293130, 292120, 291750, 292010, 292140, 293305, 293310, 293315, 293060, 292937, 292170, 290510, 292335, 292593, 292980, 290550, 293245, 290687]</t>
+  </si>
+  <si>
+    <t>[354720, 352480, 352965, 354025, 354570, 354765, 352910, 355695, 353520, 351420, 354900, 350260, 353590, 351385, 350395, 355580]</t>
+  </si>
+  <si>
+    <t>[313505, 314085, 313925, 313510, 314505, 312430, 317103, 314290, 314100, 315220, 316695, 315450, 311547, 312733, 314655]</t>
+  </si>
+  <si>
+    <t>[314915, 311783, 310825, 313520, 313210]</t>
+  </si>
+  <si>
+    <t>[352000, 352290, 350530, 350790, 350680, 352200, 350730, 355470, 352530, 351410, 352980, 350520]</t>
+  </si>
+  <si>
+    <t>[290310, 290950, 292490, 290060, 290195, 291870, 291760, 292790, 291510, 291000, 292280, 291390, 291520, 291905, 290370, 292040, 292050, 291670, 291800, 291290, 291420, 291430, 291690, 291570, 291830, 290430]</t>
+  </si>
+  <si>
+    <t>[352450, 355715, 350020, 353990, 353960, 355535, 355570, 353140, 353270, 352950, 352570]</t>
+  </si>
+  <si>
+    <t>[316100, 314470, 310600, 315570, 313620]</t>
+  </si>
+  <si>
+    <t>[313753, 313630, 310855]</t>
+  </si>
+  <si>
+    <t>[290720, 291840, 290990, 293200, 292600, 293077, 292440, 290682, 293020, 290590]</t>
+  </si>
+  <si>
+    <t>[314080, 312738, 315010, 311620, 311590, 313670, 316750, 310610, 315540, 315860, 312500, 311960]</t>
+  </si>
+  <si>
+    <t>[355650, 352520, 352590, 352400, 350960, 350840, 352730]</t>
+  </si>
+  <si>
+    <t>[120033, 120035, 120039, 120042, 120020, 120060, 120030]</t>
+  </si>
+  <si>
+    <t>[280740, 280580, 280710, 280550, 280620, 280350]</t>
+  </si>
+  <si>
+    <t>[150178, 150309, 150506, 150795, 150380, 150810]</t>
+  </si>
+  <si>
+    <t>[316040, 314890, 310420, 313720, 313530]</t>
+  </si>
+  <si>
+    <t>[350210, 351780, 353320, 352650, 353740, 352044, 352300, 353010, 355255, 353210, 351100, 355230]</t>
+  </si>
+  <si>
+    <t>[420610, 421700, 420280, 421545, 420395, 420620, 420940, 421560, 421870, 421840, 420720, 420880, 421490, 421710, 421265, 420150, 421240, 420730]</t>
+  </si>
+  <si>
+    <t>[311460, 313450, 313870, 314460, 313040, 315470, 314990, 313430, 313080, 313820]</t>
+  </si>
+  <si>
+    <t>[315840, 312290, 310440, 313800, 311530, 313260, 314670, 313840, 315410, 310460]</t>
+  </si>
+  <si>
+    <t>[310720, 313860, 310680, 315590, 310280, 314540, 315727, 313850, 310360, 314780, 315930, 314940, 310750]</t>
+  </si>
+  <si>
+    <t>[351240, 352690, 351515, 352140]</t>
+  </si>
+  <si>
+    <t>[260490, 260890, 260270, 260910, 260400, 261550, 261050, 260540, 260415, 261060, 261450, 260810, 260950, 261210, 260970, 260845, 260850, 261618, 260220, 261630]</t>
+  </si>
+  <si>
+    <t>[350880, 352710, 355590, 351720, 354160, 351700, 354010, 354460]</t>
+  </si>
+  <si>
+    <t>[352040, 351050, 355540, 355070]</t>
+  </si>
+  <si>
+    <t>[110080, 110020, 110033, 110010, 110110]</t>
+  </si>
+  <si>
+    <t>[351300, 351500, 352620, 355280, 354995, 351510, 352220, 355645]</t>
+  </si>
+  <si>
+    <t>[130115, 130310, 130185, 130380, 130030, 130255, 130353, 130260, 130356, 130040, 130360, 130110]</t>
+  </si>
+  <si>
+    <t>[313930, 314225, 316245, 314270, 313695]</t>
+  </si>
+  <si>
+    <t>[316805, 313867, 315790, 310030, 315415, 313120, 314400, 312352, 313770, 311600, 315190, 311740, 310205, 314053, 316360, 313940, 315350, 316760, 313950, 316255, 314090, 315890, 311290]</t>
+  </si>
+  <si>
+    <t>[316257, 314467, 314150, 313960, 316105, 311570, 312210, 313180]</t>
+  </si>
+  <si>
+    <t>[355330, 354630, 354910, 350030, 350040, 355640, 354810, 351518]</t>
+  </si>
+  <si>
+    <t>[150630, 150790, 150250, 150570, 150030, 150640, 150770, 150200, 150490]</t>
+  </si>
+  <si>
+    <t>[150180, 150310, 150280, 150450, 150580, 150070, 150110]</t>
+  </si>
+  <si>
+    <t>[353410, 352900, 350980, 352780, 354200, 353450, 351660, 351670, 350140, 351810, 352580, 350150, 355660, 351565, 354000, 353370, 355550, 351470, 351730]</t>
+  </si>
+  <si>
+    <t>[420360, 421003, 421915, 421917, 420900, 420005, 420390, 420520, 420400, 420920, 421180, 420670, 420287, 420415, 420680, 420040, 421850, 421985, 421105, 420860]</t>
+  </si>
+  <si>
+    <t>[320130, 320520, 320010, 320270, 320530, 320250, 320290, 320170, 320313, 320316, 320060, 320190, 320450, 320455, 320460, 320334, 320220, 320240, 320115, 320500, 320245, 320506, 320510]</t>
+  </si>
+  <si>
+    <t>[150080, 150150, 150442, 150635, 150140]</t>
+  </si>
+  <si>
+    <t>[330250, 330285, 330510, 330414, 330320, 330350, 330227, 330455, 330200, 330170, 330555, 330045]</t>
+  </si>
+  <si>
+    <t>[150275, 150020, 150820, 150700, 150190, 150800, 150260, 150710, 150650]</t>
+  </si>
+  <si>
+    <t>[330560, 330490, 330270, 330190, 330575, 330330, 330430]</t>
+  </si>
+  <si>
+    <t>[150660, 150405, 150410, 150796, 150290, 150550, 150812, 150430, 150307, 150440, 150320, 150720, 150340, 150345, 150350, 150095, 150740, 150230, 150746, 150495, 150240, 150760]</t>
+  </si>
+  <si>
+    <t>[311650, 313680, 313200, 314200, 314330, 312735]</t>
+  </si>
+  <si>
+    <t>[314210, 314820, 310310, 312490, 316140, 314220, 317140, 310550, 314390, 316443, 315645]</t>
+  </si>
+  <si>
+    <t>[130400, 130440, 130190, 130200, 130395, 130430]</t>
+  </si>
+  <si>
+    <t>[510020, 510310, 510185, 510718, 510385, 510706, 510617, 510270]</t>
+  </si>
+  <si>
+    <t>[171488, 170210, 171395, 170307, 170215, 171720, 171630, 171886, 170384, 172208, 172210, 170770, 170388, 170900, 170130, 170650, 170300]</t>
+  </si>
+  <si>
+    <t>[510787, 510885, 510726, 510345, 510795, 510130, 510263, 510170, 510685, 510623]</t>
+  </si>
+  <si>
+    <t>[330400, 330630, 330440, 330411, 330412, 330030, 330225, 330450, 330610, 330420, 330040, 330395]</t>
+  </si>
+  <si>
+    <t>[420290, 420515, 421510, 421320, 420170, 421820, 420590, 420270, 420240, 420750, 420630, 420220, 420125, 421470]</t>
+  </si>
+  <si>
+    <t>[314430, 311370, 316670]</t>
+  </si>
+  <si>
+    <t>[420130, 420580, 420845, 420205, 420910, 421620]</t>
+  </si>
+  <si>
+    <t>[521350, 520490, 520530, 522108, 520830]</t>
+  </si>
+  <si>
+    <t>[520670, 521830, 520396, 520940, 520080, 521490, 522068, 522070, 521270, 521980, 520990]</t>
+  </si>
+  <si>
+    <t>[330210, 330115, 330470, 330310, 330090, 330410, 330060, 330220, 330513, 330230, 330615, 330300, 330205, 330015]</t>
+  </si>
+  <si>
+    <t>[510337, 510285, 510190, 510515, 510517, 510325, 510140]</t>
+  </si>
+  <si>
+    <t>[521377, 521410, 522145, 522020, 520357, 521960, 521800, 520810, 520750, 520465, 521525, 521308, 521405]</t>
+  </si>
+  <si>
+    <t>[330240, 330500, 330475, 330093, 330415, 330480, 330100, 330140]</t>
+  </si>
+  <si>
+    <t>[351200, 352420, 351210, 350090, 353390, 351790, 350930, 350550, 355190, 351740]</t>
+  </si>
+  <si>
+    <t>[510785, 510530, 510788, 510631, 510035]</t>
+  </si>
+  <si>
+    <t>[510880, 510320, 510455, 510619, 510621, 510558]</t>
+  </si>
+  <si>
+    <t>[352930, 351010, 351400, 355370, 354650]</t>
+  </si>
+  <si>
+    <t>[280450, 280260, 280420, 280540, 280240, 280560, 280310, 280120, 280220]</t>
+  </si>
+  <si>
+    <t>[280480, 280610, 280130, 280330, 280460, 280720, 280400, 280530, 280660, 280150, 280250, 280190]</t>
+  </si>
+  <si>
+    <t>[421507, 421775, 421140, 421145, 420895, 421290, 421420, 420785, 420665, 420410, 420543, 421569, 421315, 420420, 420165, 421187, 420050, 420435, 420310, 420055, 420440, 421210, 421600, 421755, 420470, 420475, 421885]</t>
+  </si>
+  <si>
+    <t>[521030, 521020, 521160, 521720, 520170, 520235, 520710, 521200, 521520, 520340, 520310, 520760, 521370, 521340, 521565, 520090]</t>
+  </si>
+  <si>
+    <t>[521570, 520260, 520420, 522150, 521640, 520393, 520780, 521900, 520015, 522005, 521590, 520570, 522010]</t>
+  </si>
+  <si>
+    <t>[510720, 510562, 510343, 510250, 510125, 510450, 510395, 510710, 510775, 510682, 510523, 510715]</t>
+  </si>
+  <si>
+    <t>[314560, 311400, 314770, 315990, 316120, 311450]</t>
+  </si>
+  <si>
+    <t>[261255, 260200, 260110, 261040, 260530, 261430, 260630, 261560, 260730, 261245, 260990]</t>
+  </si>
+  <si>
+    <t>[355460, 353380, 350630, 351015, 355720, 355050, 354540, 351950, 354640, 354320, 352090, 353470, 351519]</t>
+  </si>
+  <si>
+    <t>[314000, 314610, 313190]</t>
+  </si>
+  <si>
+    <t>[311545, 313230, 311300, 314630]</t>
+  </si>
+  <si>
+    <t>[260480, 260870, 261000, 261650, 261140, 261150, 260520, 261290, 261420, 260140, 260150, 260920, 260795, 261180, 260420, 261190, 260040, 260820, 261340, 261485, 260590, 260090]</t>
+  </si>
+  <si>
+    <t>[315140, 313830, 311760, 314580, 316310, 314710, 314520, 313020]</t>
+  </si>
+  <si>
+    <t>[316294, 314790, 310760, 310190, 314510, 311440, 312630, 316220, 313375]</t>
+  </si>
+  <si>
+    <t>[312070, 316680, 316170, 317100, 315340, 313710, 314800, 317075, 313750, 312890, 312860]</t>
+  </si>
+  <si>
+    <t>[312480, 314310, 313160, 310010, 311930, 312790, 315640, 314810, 312350]</t>
+  </si>
+  <si>
+    <t>[291810, 290020, 292420, 292710, 291140, 292400, 290770, 291990, 292760]</t>
+  </si>
+  <si>
+    <t>[312235, 310100, 312245, 314870, 310270]</t>
+  </si>
+  <si>
+    <t>[210400, 210594, 210596, 210820, 210600, 210570, 210890, 210193, 210580, 211223, 210520, 211163, 211167]</t>
+  </si>
+  <si>
+    <t>[260515, 260875, 260300, 261260, 260980, 260020, 261110]</t>
+  </si>
+  <si>
+    <t>[311205, 314860, 316280, 312695, 314840, 316410, 316350]</t>
+  </si>
+  <si>
+    <t>[210370, 210083, 210980, 210310, 210312, 210825, 211178, 211240, 210860, 211245, 210190, 210927, 210130, 210840, 210680, 210905, 210490]</t>
+  </si>
+  <si>
+    <t>[354400, 351040, 353090, 354210, 351170, 351490, 355040, 354700, 350060, 353870, 354515]</t>
+  </si>
+  <si>
+    <t>[312960, 315213, 315120, 315760, 313810, 317080, 310940]</t>
+  </si>
+  <si>
+    <t>[521730, 520580, 520485, 520551, 522119, 520840, 520010, 520110, 520815, 520030]</t>
+  </si>
+  <si>
+    <t>[317060, 315050, 312810, 316430, 315150, 311280, 312340]</t>
+  </si>
+  <si>
+    <t>[421500, 421220, 421030, 421830, 420330, 420810, 421580, 421360, 421010, 420213, 420790, 421110, 420380]</t>
+  </si>
+  <si>
+    <t>[220669, 220770, 220200, 220265, 220270, 220272, 220208, 220465, 220570, 220253, 220191]</t>
+  </si>
+  <si>
+    <t>[352640, 354050, 350690, 355010, 350750, 355465, 353610, 351230, 350230, 350360, 354105, 353750, 352350]</t>
+  </si>
+  <si>
+    <t>[354425, 353020, 355430, 351535]</t>
+  </si>
+  <si>
+    <t>[315400, 315020, 316556, 310040, 310570, 316340, 315210, 312270, 313550, 316630, 310230, 314585, 315740, 315490, 312170, 310250, 315500, 316010, 316400, 312820, 317050]</t>
+  </si>
+  <si>
+    <t>[291072, 292770, 290340, 291465, 291530, 291180, 291630, 292530]</t>
+  </si>
+  <si>
+    <t>[312450, 310790, 311050, 314380, 316557, 313360, 313490, 311060, 316440, 316580, 310830, 316980, 311990, 315960, 310970, 313150, 312510, 311360, 316740, 316230, 314440, 312920, 313060, 311780, 314340, 314600, 316905, 316910, 311790, 315250, 312440, 310910]</t>
+  </si>
+  <si>
+    <t>[315180, 315920, 310260, 311030, 310140, 312990]</t>
+  </si>
+  <si>
+    <t>[210560, 210275, 211174, 210462, 210440, 210470, 210380, 210450, 210420, 211125, 211030, 210910, 211070, 210460, 211230, 210975]</t>
+  </si>
+  <si>
+    <t>[280640, 280160, 280070, 280730, 280010, 280490, 280110, 280270, 280430, 280690, 280340, 280020, 280470, 280440, 280570, 280380]</t>
+  </si>
+  <si>
+    <t>[260610, 261640, 260105, 261130, 260760, 260005, 260775, 261160, 260790, 260545, 260290, 260680, 260940, 261070, 260440, 260960, 260450, 260720, 260345, 261370]</t>
+  </si>
+  <si>
+    <t>[130180, 130150, 130195, 130100, 130165, 130140]</t>
+  </si>
+  <si>
+    <t>[130240, 130410, 130090, 130350, 130070]</t>
+  </si>
+  <si>
+    <t>[431120, 432149, 431912, 431402, 431532, 430637, 430010, 431550, 432065, 431940, 431690, 431053, 430670, 431310, 430800, 431447, 431960, 432345, 432220, 431843, 431075, 430840]</t>
+  </si>
+  <si>
+    <t>[430465, 431810, 431110, 431303, 431113, 431210, 431980, 432237, 431055, 430290, 431740]</t>
+  </si>
+  <si>
+    <t>[431171, 431175, 431640, 431530, 430187, 432240, 431697, 431060, 431830, 430040, 431710]</t>
+  </si>
+  <si>
+    <t>[431173, 432166, 431177, 431244, 430655, 432143, 431065, 432150, 432183, 430105, 432380, 430463]</t>
+  </si>
+  <si>
+    <t>[432160, 430467, 431365, 432135, 430471, 431760, 430545, 431250, 430163, 431350, 431033]</t>
+  </si>
+  <si>
+    <t>[430360, 431010, 432170, 431820, 431405, 431600, 431575, 432120]</t>
+  </si>
+  <si>
+    <t>[430087, 430760, 431080, 431306, 431848, 431340, 431247, 430640, 431514, 431695, 430390, 431990, 431480, 431162, 431870]</t>
+  </si>
+  <si>
+    <t>[432000, 432225, 431650, 430468, 431240, 431337, 432200, 430955, 431403, 431179, 431950, 430770, 431861, 430165, 432085, 430265, 430460, 431935]</t>
+  </si>
+  <si>
+    <t>[430085, 430605, 430350, 430110, 430880, 432035, 430517, 432055, 430650, 430270, 430535, 430544, 430930, 430676, 431198, 430175, 431840, 432110, 430190, 431225]</t>
+  </si>
+  <si>
+    <t>[431490, 430310, 430920, 432300, 430060, 430905]</t>
+  </si>
+  <si>
+    <t>[431750, 431630, 430865, 431890, 431510, 431770, 431647, 430250, 431915, 430635, 431920, 431800, 432057, 430520, 430783, 431937, 431455, 430693, 430950, 432234, 431595, 431217, 432375, 430330]</t>
+  </si>
+  <si>
+    <t>[430560, 431645, 430222, 431535, 431087, 430223, 430610, 431670, 431000, 431643, 430845, 432030]</t>
+  </si>
+  <si>
+    <t>[430600, 431115, 432023, 431390, 430500, 431780, 431910, 431020, 430258, 430400, 431041, 430020, 431430, 430150, 430540, 431973, 431333, 430570, 430970, 430587]</t>
+  </si>
+  <si>
+    <t>[430220, 431500, 431505, 431507, 432032, 430370, 431790, 432180, 430900, 431930, 431040, 431301, 430030, 430673, 432210, 430045, 430430, 432230, 431720, 431849, 431342, 430960]</t>
+  </si>
+  <si>
+    <t>[430850, 432132, 430340, 430730, 432140, 430607, 432147, 431380, 432020, 430745, 430237, 430632, 432310, 431160, 432190, 431050, 431445, 431449, 432350, 430050, 431590, 430185, 431470, 430064, 431344, 432370]</t>
+  </si>
+  <si>
+    <t>[430720, 430090, 430613, 430870, 430485, 432290, 430755, 432163, 431270, 430890, 431531, 430380, 430511, 431413, 432060, 431555, 431046, 430537, 430155, 430805, 431190, 430170, 431070, 431200, 431970, 430695, 430697, 430825, 430700, 430192, 431090, 431478, 430205]</t>
+  </si>
+  <si>
+    <t>[431235, 430597, 430470, 431755, 430355, 431127, 430490, 431262, 431775, 431265, 431267, 430885, 430630, 432040, 431275, 432050, 431410, 431805, 432320, 431180, 432340, 430550, 430047, 431213, 430705, 431477, 430585, 432255]</t>
+  </si>
+  <si>
+    <t>[431360, 430980, 430990, 431130, 430495, 431660, 431795, 430005, 431673, 431170, 432335, 432090, 432218, 431842, 430180, 430320, 430066, 431860, 431220, 430462]</t>
+  </si>
+  <si>
+    <t>[432100, 430055, 431242, 430410, 430830, 432080, 431057, 432146, 430995, 431125, 432215, 430200, 430140, 430750]</t>
+  </si>
+  <si>
+    <t>[431620, 430590, 430215, 432010, 431370, 431642, 431142, 430642, 430515, 430260, 431540, 432185, 431295, 431936, 430912, 430530, 432195, 430692, 431845, 431085, 431346, 430195, 430580, 431349, 431610, 431230]</t>
+  </si>
+  <si>
+    <t>[430466, 431880, 431245, 430107, 430512, 430130, 431417, 431420, 431560, 430543, 431440, 431700, 431450, 431460, 432232, 431850, 430063, 431730, 430450, 430710, 431100]</t>
+  </si>
+  <si>
+    <t>[430435, 430660, 431150, 430160, 430003, 430965]</t>
+  </si>
+  <si>
+    <t>[430440, 430510, 431442, 431320, 431164, 430910]</t>
+  </si>
+  <si>
+    <t>[431237, 431112, 430740, 431446, 431862, 430230, 432250, 431261, 430367]</t>
+  </si>
+  <si>
+    <t>[430593, 430210, 430595, 431238, 430860, 430480, 430225, 432280, 431517, 431400, 431280, 431290, 430786, 432330, 430925, 430940, 431453, 431454, 431330, 431844, 432360, 432235, 431725]</t>
+  </si>
+  <si>
+    <t>[430080, 431043, 430820, 430790, 431975, 431335, 430057, 431308, 430810, 430235, 431900, 432254]</t>
+  </si>
+  <si>
+    <t>[430690, 432070, 430120, 430280, 431339, 431406, 430513, 431123, 432026, 430300, 430781, 430975]</t>
+  </si>
+  <si>
+    <t>[431680, 432067, 432260, 430915, 431395, 430957, 432270, 431407, 431215, 431570, 430420, 432252, 432253]</t>
+  </si>
+  <si>
+    <t>[430469, 430100, 431513, 431515, 430620, 432285, 431260, 431520, 432162, 431140, 430245, 432045, 430645, 431030, 431545, 431675, 431300, 430675, 430680, 431580, 431971, 431205, 431846, 430070, 430583, 430843, 430461]</t>
+  </si>
+  <si>
+    <t>[430240, 430780, 432130, 430807, 432145, 431475, 431415, 432377, 431036, 430558]</t>
+  </si>
+  <si>
+    <t>[354580, 353180, 351905, 351907, 355620, 355240, 350380, 353710, 351280, 353200, 352050, 353340, 350160, 352340, 352470, 355670, 350950, 354800, 353650]</t>
+  </si>
+  <si>
+    <t>[311840, 312737, 313410, 315430, 310220, 315950, 312083, 310110]</t>
+  </si>
+  <si>
+    <t>[292290, 291075, 290790, 290920, 292650, 290160, 291185, 292305, 290035, 293076, 292660, 292310, 290265, 290780, 292380]</t>
+  </si>
+  <si>
+    <t>[150560, 150690, 150500, 150090, 150540, 150220, 150830, 150160, 150610, 150611, 150803, 150195, 150170, 150747, 150620, 150655]</t>
+  </si>
+  <si>
+    <t>[351270, 352360, 352110, 354670, 354390, 350200]</t>
+  </si>
+  <si>
+    <t>[130080, 130330, 130014, 130170, 130270]</t>
+  </si>
+  <si>
+    <t>[130083, 130120, 130250, 130063, 130320, 130130, 130008, 130010]</t>
+  </si>
+  <si>
+    <t>[355360, 355080, 351080, 350870, 354970, 353050, 352380, 351390]</t>
+  </si>
+  <si>
+    <t>[520960, 520929, 521120, 520250, 521925, 521220, 521483, 521100, 521390, 521295, 521040, 520753, 520085, 520215, 521400, 520890, 520380]</t>
+  </si>
+  <si>
+    <t>[210500, 210920, 211020, 210125, 210510, 210960, 211027, 210710, 210170, 210940, 210237, 210110]</t>
+  </si>
+  <si>
+    <t>[353440, 350570, 354730, 351060, 352500, 353910, 352250]</t>
+  </si>
+  <si>
+    <t>[260160, 260930, 261220, 261610, 260430, 261520, 261400]</t>
+  </si>
+  <si>
+    <t>[292740, 293320, 292975, 291920, 292950, 292920, 290650, 291610, 292860, 291992]</t>
+  </si>
+  <si>
+    <t>[355490, 354660, 353284, 354610, 354450, 354740]</t>
+  </si>
+  <si>
+    <t>[210465, 210850, 210690, 210177, 211172, 210200, 210990, 210515, 210870, 211000, 211227, 211102, 210047]</t>
+  </si>
+  <si>
+    <t>[293030, 292905, 292810, 291735, 290610, 293075, 290930, 292820, 290390, 293015, 290810, 290910]</t>
+  </si>
+  <si>
+    <t>[316450, 315820, 310060, 313655]</t>
+  </si>
+  <si>
+    <t>[292870, 290830, 292240, 292250, 292130, 291880, 290730, 292910, 290100, 290230, 291780, 293317, 292940, 291020, 291030, 293210, 292575, 291685, 291820, 292850, 292730, 292220]</t>
+  </si>
+  <si>
+    <t>[314570, 310330, 316070]</t>
+  </si>
+  <si>
+    <t>[290400, 292990, 291300, 291930, 292350, 292430, 292303, 291440, 293080, 290010, 292190]</t>
+  </si>
+  <si>
+    <t>[290180, 290600, 292460, 292525, 291085, 293010, 291700, 290135, 291770]</t>
+  </si>
+  <si>
+    <t>[421505, 421890, 420417, 420260, 420325, 420100, 421895, 420930, 420455, 421189, 421680, 421330, 421650, 420340, 420243, 421205, 421175, 420250]</t>
+  </si>
+  <si>
+    <t>[261570, 260740, 261350, 260392, 261390, 260560, 260180, 260340, 260570, 261247]</t>
+  </si>
+  <si>
+    <t>[220192, 221060, 220070, 220455, 221000, 220553, 221035, 220556, 220335, 221135, 220211, 220245, 220375, 220345, 220250, 220955, 220285, 220535]</t>
+  </si>
+  <si>
+    <t>[521280, 520552, 521487, 522160, 520082, 521460, 520980, 520470, 520055]</t>
+  </si>
+  <si>
+    <t>[330080, 330530, 330050, 330340, 330245, 330150, 330110, 330120, 330185, 330570, 330160, 330515, 330580, 330390, 330460, 330590]</t>
+  </si>
+  <si>
+    <t>[292610, 290327, 290840, 293150, 292895, 290210, 292265, 293300, 292150, 290360, 293050, 292800, 290040, 291910, 293190, 292580, 292590, 290680, 291070]</t>
+  </si>
+  <si>
+    <t>[310240, 311750, 316710, 316650, 316020]</t>
+  </si>
+  <si>
+    <t>[310020, 311560, 313100, 314640, 312720, 310700, 310320, 310960, 316720, 315200, 312640, 314690, 315850, 310990, 314960, 311890, 311250, 315360, 313570, 310500, 315370, 314350, 313970, 314740]</t>
+  </si>
+  <si>
+    <t>[352390, 354060, 355220, 355350, 350115, 351030, 350275, 352840, 352585, 350290, 354520, 354530, 351970, 352100, 350700, 353780, 355700, 355060, 355450, 353790]</t>
+  </si>
+  <si>
+    <t>[170240, 170560, 171620, 171525, 171780, 170700, 171215, 171800, 171515, 170040, 171865, 172090, 170555, 172093, 170270]</t>
+  </si>
+  <si>
+    <t>[521225, 521130, 522155, 521930, 520013, 521880, 520410, 520430, 520145, 522040, 521971, 521300, 521805, 521080, 520505, 521850, 521630, 521375]</t>
+  </si>
+  <si>
+    <t>[522050, 520547, 521190, 521645, 521810, 521940, 520725, 520150, 520440, 521310]</t>
+  </si>
+  <si>
+    <t>[510336, 510500, 510757, 510380, 510330, 510675, 510835, 510550, 510618, 510268]</t>
+  </si>
+  <si>
+    <t>[320260, 320265, 320140, 320020, 320280, 320030, 320420, 320040, 320300, 320430, 320050, 320180, 320310, 320440, 320070, 320200, 320332, 320340, 320480, 320230, 320110, 320370, 320503, 320120, 320380, 320255]</t>
+  </si>
+  <si>
+    <t>[521600, 520993, 521380, 520390, 520425, 520910, 520050, 520915, 520020, 521210, 520350, 521150]</t>
+  </si>
+  <si>
+    <t>[140028, 140047, 140050, 140020, 140023, 140060]</t>
+  </si>
+  <si>
+    <t>[355680, 355365, 355690, 355310, 355440, 350610, 355320, 353150]</t>
+  </si>
+  <si>
+    <t>[510729, 510480, 510740, 510360, 510630, 510120, 510760, 510637, 510520, 510779, 510267, 510030, 510420, 510040, 510810, 510060, 510700, 510704, 510460]</t>
+  </si>
+  <si>
+    <t>[315970, 311430, 314120, 310380, 316210, 316890, 315550]</t>
+  </si>
+  <si>
+    <t>[353280, 351750, 353030, 355340, 353420, 350480, 353040, 353300, 353660, 351130, 354080, 354980, 351940, 353500, 353250, 355560, 351980, 352115, 353400, 350460]</t>
+  </si>
+  <si>
+    <t>[311520, 311970, 315270, 313000, 315610, 313740, 312300, 310800, 316880, 316530, 314450, 316500, 315733, 315030, 313910, 316250, 315420, 310590]</t>
+  </si>
+  <si>
+    <t>[310690, 316290, 312130, 314020, 314950, 315620, 316560, 312850, 313980]</t>
+  </si>
+  <si>
+    <t>[210592, 210180, 210790, 211110, 210150, 210730, 210350, 210670, 210800, 210545, 210770, 210230, 211190, 211065, 211195]</t>
+  </si>
+  <si>
+    <t>[314760, 312080, 316700, 313780, 314550, 311480, 316490, 314190, 316370, 313300, 312280, 311770, 310490, 313310, 316640, 310120, 316780, 317170, 310130, 311410, 312050, 313590, 315260, 311550]</t>
+  </si>
+  <si>
+    <t>[210945, 210020, 211120, 211130, 210750]</t>
+  </si>
+  <si>
+    <t>[521090, 521860, 521870, 521486, 522015, 521890, 521385, 522028, 522157, 520495, 520500, 521015, 522170, 520640, 521935, 521690, 520540, 520945, 521970, 521470]</t>
+  </si>
+  <si>
+    <t>[520320, 521060, 521180, 521945, 522230, 521560, 521305, 520860]</t>
+  </si>
+  <si>
+    <t>[355030]</t>
+  </si>
+  <si>
+    <t>[313480, 313290, 314320, 316470, 315290, 316510]</t>
+  </si>
+  <si>
+    <t>[221120, 221063, 220080, 220115, 220890]</t>
+  </si>
+  <si>
+    <t>[316800, 314465, 315560, 313065, 310665, 317065, 314345, 316045, 316270, 312087]</t>
+  </si>
+  <si>
+    <t>[150375, 150503, 150100, 150805, 150360, 150619]</t>
+  </si>
+  <si>
+    <t>[290080, 290690, 291845, 292550, 291560, 292200, 292300, 293325, 292110, 293135, 291280, 291600, 291890]</t>
+  </si>
+  <si>
+    <t>[510624, 510305, 510370, 510850, 510724, 510790, 510792, 510830, 510800, 510452, 510454, 510776, 510525, 510622]</t>
+  </si>
+  <si>
+    <t>[313920, 314530, 312675, 313700, 310470, 314535, 315240, 316555, 310285, 316860, 314620]</t>
+  </si>
+  <si>
+    <t>[211090, 210660, 211220, 210780]</t>
+  </si>
+  <si>
+    <t>[150400, 150210, 150470, 150120, 150130, 150010, 150520, 150330, 150460]</t>
+  </si>
+  <si>
+    <t>[130210, 130280, 130220, 130002, 130420, 130426]</t>
+  </si>
+  <si>
+    <t>[353630, 353700, 351620, 354310, 354950, 352370, 354360, 351320, 352540, 354270]</t>
+  </si>
+  <si>
+    <t>[316930, 316520, 311070, 316080, 311090, 311390]</t>
+  </si>
+  <si>
+    <t>[500290, 500100, 500230, 500780, 500755, 500020, 500630, 500440, 500830, 500190]</t>
+  </si>
+  <si>
+    <t>[316940, 310710, 315830, 313050, 311870]</t>
+  </si>
+  <si>
+    <t>[353600, 354180, 354380, 355500, 351920, 350580, 351900, 350335]</t>
+  </si>
+  <si>
+    <t>[314180, 316970, 313835, 310445, 317107, 313652, 311610, 311230]</t>
+  </si>
+  <si>
+    <t>[311140, 315690, 311820, 317010, 311730, 310070, 317110, 312125]</t>
+  </si>
+  <si>
+    <t>[316960, 314500, 310375, 314280, 311500, 310350, 313070, 315280, 317020]</t>
+  </si>
+  <si>
+    <t>[312840, 312330, 317200, 316570, 315310, 312880, 314160, 316730, 315580, 316990, 312900, 312400, 310870, 316900, 315630, 311670, 316790, 316150, 315130, 312190]</t>
+  </si>
+  <si>
+    <t>[310945, 310820, 314437, 317047, 314700, 312620, 317040, 310930, 310450, 315445, 312247, 311615]</t>
+  </si>
+  <si>
+    <t>[354625, 350590, 354790, 351090, 350100, 350940, 350780]</t>
+  </si>
+  <si>
+    <t>[220385, 220995, 220280, 220965, 220937, 220490, 221097, 220207, 220210, 220277, 220950, 221080, 220155, 220700]</t>
+  </si>
+  <si>
+    <t>[110008, 110149, 110150]</t>
+  </si>
+  <si>
+    <t>[110026, 110060, 110094, 110002, 110070, 110040, 110140, 110045, 110013]</t>
+  </si>
+  <si>
+    <t>[351140, 355300, 350310, 350055, 350500, 353880, 353580, 351260, 355120, 350450, 351540, 351925, 355380, 352180, 352280, 355420, 352860]</t>
+  </si>
+  <si>
+    <t>[354820, 353800, 354860, 353230, 355410, 354230, 352630, 355000, 350970, 355480]</t>
+  </si>
+  <si>
+    <t>[510560, 510626, 510410, 510642, 510805]</t>
+  </si>
+  <si>
+    <t>[352610, 353720, 352042, 352330, 352460, 355180, 352990, 350540, 350925, 350990, 352120, 353620, 354260, 351480, 352030]</t>
+  </si>
+  <si>
+    <t>[220800, 220420, 220935, 220940, 220173, 221070, 220430, 220435, 220180, 220820, 221093, 220327, 220720, 220209, 220595, 220340, 220213, 220985, 220605, 220095, 220480, 220865, 220755, 220500, 221020, 221150, 220255, 220515, 220005, 221030, 221160, 220777, 220650, 220520, 220780, 221037, 220910, 221170, 220025, 220027, 220157, 220415]</t>
+  </si>
+  <si>
+    <t>[220960, 221130, 220810, 221038, 220559, 220400, 220690, 220915, 221140, 220117, 220470, 220090, 220860, 220350]</t>
+  </si>
+  <si>
+    <t>[510680, 510794, 510627, 510510]</t>
+  </si>
+  <si>
+    <t>[220170, 220560, 220450, 221090, 220198, 221095, 220970, 220590, 220855, 220600, 220730, 220735, 220225, 220100, 220230, 221010, 220887, 220380, 220510, 220900, 220390, 221039, 220785, 220530, 220793, 220410, 220795, 220670]</t>
+  </si>
+  <si>
+    <t>[293120, 292260, 293350, 293160, 293290, 290540, 291120, 291345, 291730, 292275, 290580, 292467]</t>
+  </si>
+  <si>
+    <t>[316200, 312360, 317070, 314260, 311900]</t>
+  </si>
+  <si>
+    <t>[317120, 313760, 316295, 311787, 314930, 315900, 314110]</t>
+  </si>
+  <si>
+    <t>[210240, 211170, 210760, 211050, 210250, 210830, 211280, 210135, 210745, 210650, 211100]</t>
+  </si>
+  <si>
+    <t>[290689, 292500, 291995, 292510, 290350, 292145, 290870, 292665, 293180, 290120, 293330, 290515, 290900, 292570, 290395, 291040, 290670, 290290, 292470]</t>
+  </si>
+  <si>
+    <t>[314880, 311170, 310370, 317130, 311020, 314830, 316850, 316380, 315230]</t>
+  </si>
+  <si>
+    <t>[351680, 355710, 350180, 351290, 351590, 350120, 352810, 351690, 353100, 353260, 354030, 351070, 354420, 353625, 355610, 355130, 352830]</t>
+  </si>
+  <si>
+    <t>[421910, 420253, 420768, 420517, 420010, 421165, 420530, 420917, 421690, 421950, 421055, 421185, 421575, 420560, 420945, 421970, 421340, 420445, 421610, 421227, 420350]</t>
+  </si>
+  <si>
+    <t>[150172, 150085, 150060, 150445, 150835, 150548, 150780, 150590, 150815]</t>
+  </si>
+  <si>
+    <t>[110145, 110050, 110090, 110028, 110029, 110001, 110037, 110014]</t>
+  </si>
+  <si>
+    <t>[210467, 210565, 210087, 211400, 210632, 210055, 210923, 210315, 210317, 210637, 210735, 210290, 210260, 210197, 211003, 210620, 210430]</t>
+  </si>
+  <si>
+    <t>[314625, 315650, 312707, 314537, 315700, 315737]</t>
+  </si>
+  <si>
+    <t>[420450, 421635, 421060, 420650, 421740, 420210, 420890]</t>
+  </si>
+  <si>
+    <t>[312705, 314850, 313890, 310660, 317030, 310090, 312015, 315765]</t>
+  </si>
+  <si>
+    <t>[160005, 160015, 160021, 160053, 160023, 160025, 160030]</t>
+  </si>
+  <si>
+    <t>[160070, 160010, 160050, 160020, 160055]</t>
+  </si>
+  <si>
+    <t>[160080, 160040, 160027, 160060]</t>
   </si>
 </sst>
 </file>

</xml_diff>